<commit_message>
Domain renewals (Relaxatub and Airylea)
</commit_message>
<xml_diff>
--- a/clients/Domains.xlsx
+++ b/clients/Domains.xlsx
@@ -457,7 +457,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -537,13 +537,6 @@
       <u/>
       <sz val="11"/>
       <color indexed="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -649,9 +642,9 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -823,9 +816,6 @@
     <xf numFmtId="15" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -837,10 +827,10 @@
     <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="14" fillId="11" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="13" fillId="11" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1164,10 +1154,10 @@
   <dimension ref="A1:V30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1176,7 +1166,7 @@
     <col min="2" max="2" width="33.5703125" style="63" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" style="65" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.5703125" style="65" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="83" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="82" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" style="74" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" style="74" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="46.5703125" style="74" bestFit="1" customWidth="1"/>
@@ -1263,119 +1253,137 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="64">
-        <v>1017</v>
+        <v>1010</v>
       </c>
       <c r="B2" s="63" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C2" s="65" t="s">
         <v>65</v>
       </c>
       <c r="D2" s="63" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="66">
-        <v>40857</v>
-      </c>
-      <c r="F2" s="85">
-        <v>20124</v>
-      </c>
-      <c r="G2" s="66">
-        <v>40857</v>
+        <v>14</v>
+      </c>
+      <c r="E2" s="78">
+        <v>40917</v>
+      </c>
+      <c r="F2" s="69">
+        <v>131</v>
+      </c>
+      <c r="G2" s="78">
+        <v>40917</v>
       </c>
       <c r="H2" s="67" t="str">
         <f>"Renewal of Domain and Hosting until "&amp;TEXT(G2,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 10-Nov-2011</v>
+        <v>Renewal of Domain and Hosting until 09-Jan-2012</v>
       </c>
       <c r="I2" s="67" t="str">
         <f>"Renewal of Domain "&amp;B2&amp;" until "&amp;TEXT(G2,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain westcoastexpress.net until 10-Nov-2011</v>
+        <v>Renewal of Domain onestopaberdeen.com until 09-Jan-2012</v>
       </c>
       <c r="J2" s="68" t="s">
         <v>40</v>
       </c>
       <c r="K2" s="59"/>
       <c r="L2" s="63" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="M2" s="63" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="N2" s="63" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="O2" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="P2" s="77"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="64">
+        <v>1007</v>
+      </c>
       <c r="B3" s="63" t="s">
-        <v>136</v>
+        <v>5</v>
       </c>
       <c r="C3" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="64" t="s">
-        <v>136</v>
-      </c>
-      <c r="E3" s="75">
-        <v>40857</v>
-      </c>
-      <c r="G3" s="75">
-        <v>40857</v>
+      <c r="D3" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="76">
+        <v>40992</v>
+      </c>
+      <c r="F3" s="79">
+        <v>140</v>
+      </c>
+      <c r="G3" s="76">
+        <v>40992</v>
       </c>
       <c r="H3" s="67" t="str">
         <f>"Renewal of Domain and Hosting until "&amp;TEXT(G3,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 10-Nov-2011</v>
+        <v>Renewal of Domain and Hosting until 24-Mar-2012</v>
       </c>
       <c r="I3" s="67" t="str">
         <f>"Renewal of Domain "&amp;B3&amp;" until "&amp;TEXT(G3,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain goodteaching.org until 10-Nov-2011</v>
+        <v>Renewal of Domain dsglasscraft.com until 24-Mar-2012</v>
       </c>
       <c r="J3" s="68" t="s">
         <v>40</v>
+      </c>
+      <c r="K3" s="59"/>
+      <c r="L3" s="63" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3" s="63" t="s">
+        <v>76</v>
+      </c>
+      <c r="N3" s="63" t="s">
+        <v>94</v>
+      </c>
+      <c r="O3" s="63" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="64">
-        <v>1013</v>
+        <v>1004</v>
       </c>
       <c r="B4" s="63" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="C4" s="65" t="s">
         <v>65</v>
       </c>
       <c r="D4" s="63" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="75">
-        <v>40857</v>
-      </c>
-      <c r="F4" s="71">
-        <v>10309</v>
-      </c>
-      <c r="G4" s="75">
-        <v>40857</v>
+        <v>13</v>
+      </c>
+      <c r="E4" s="67">
+        <v>41096</v>
+      </c>
+      <c r="F4" s="74">
+        <v>141</v>
+      </c>
+      <c r="G4" s="66">
+        <v>40999</v>
       </c>
       <c r="H4" s="67" t="str">
         <f>"Renewal of Domain and Hosting until "&amp;TEXT(G4,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 10-Nov-2011</v>
+        <v>Renewal of Domain and Hosting until 31-Mar-2012</v>
       </c>
       <c r="I4" s="67" t="str">
         <f>"Renewal of Domain "&amp;B4&amp;" until "&amp;TEXT(G4,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain powersoftware.com until 10-Nov-2011</v>
+        <v>Renewal of Domain midwestmarketforce.com until 31-Mar-2012</v>
       </c>
       <c r="J4" s="68" t="s">
         <v>40</v>
       </c>
       <c r="K4" s="59"/>
       <c r="L4" s="63" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="M4" s="63" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="N4" s="63" t="s">
         <v>94</v>
@@ -1386,46 +1394,46 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="64">
-        <v>1010</v>
+        <v>1004</v>
       </c>
       <c r="B5" s="63" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="C5" s="65" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D5" s="63" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="78">
-        <v>40917</v>
-      </c>
-      <c r="F5" s="69">
-        <v>131</v>
-      </c>
-      <c r="G5" s="78">
-        <v>40917</v>
+        <v>13</v>
+      </c>
+      <c r="E5" s="66">
+        <v>41116</v>
+      </c>
+      <c r="F5" s="74">
+        <v>141</v>
+      </c>
+      <c r="G5" s="66">
+        <v>40999</v>
       </c>
       <c r="H5" s="67" t="str">
         <f>"Renewal of Domain and Hosting until "&amp;TEXT(G5,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 09-Jan-2012</v>
+        <v>Renewal of Domain and Hosting until 31-Mar-2012</v>
       </c>
       <c r="I5" s="67" t="str">
         <f>"Renewal of Domain "&amp;B5&amp;" until "&amp;TEXT(G5,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain onestopaberdeen.com until 09-Jan-2012</v>
+        <v>Renewal of Domain midwestmarketforce.info until 31-Mar-2012</v>
       </c>
       <c r="J5" s="68" t="s">
         <v>40</v>
       </c>
       <c r="K5" s="59"/>
       <c r="L5" s="63" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M5" s="63" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="N5" s="63" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="O5" s="63" t="s">
         <v>95</v>
@@ -1433,234 +1441,285 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="64">
-        <v>1001</v>
+        <v>1004</v>
       </c>
       <c r="B6" s="63" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C6" s="65" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D6" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="76">
-        <v>40965</v>
+        <v>13</v>
+      </c>
+      <c r="E6" s="75">
+        <v>41165</v>
       </c>
       <c r="F6" s="74">
-        <v>138</v>
-      </c>
-      <c r="G6" s="76">
-        <v>40965</v>
+        <v>10593</v>
+      </c>
+      <c r="G6" s="66">
+        <v>40999</v>
       </c>
       <c r="H6" s="67" t="str">
         <f>"Renewal of Domain and Hosting until "&amp;TEXT(G6,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 26-Feb-2012</v>
+        <v>Renewal of Domain and Hosting until 31-Mar-2012</v>
       </c>
       <c r="I6" s="67" t="str">
         <f>"Renewal of Domain "&amp;B6&amp;" until "&amp;TEXT(G6,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain relaxatub.com until 26-Feb-2012</v>
+        <v>Renewal of Domain mwmf.co.uk until 31-Mar-2012</v>
       </c>
       <c r="J6" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="K6" s="59"/>
+      <c r="K6" s="63" t="s">
+        <v>116</v>
+      </c>
       <c r="L6" s="63" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="M6" s="63" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="N6" s="63" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="O6" s="63" t="s">
-        <v>95</v>
+        <v>93</v>
+      </c>
+      <c r="P6" s="63" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q6" s="63" t="s">
+        <v>99</v>
+      </c>
+      <c r="R6" s="63">
+        <v>3528228</v>
+      </c>
+      <c r="S6" s="80" t="s">
+        <v>113</v>
+      </c>
+      <c r="T6" s="80" t="s">
+        <v>115</v>
+      </c>
+      <c r="U6" s="72">
+        <v>38982</v>
+      </c>
+      <c r="V6" s="72">
+        <v>38989</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="64">
-        <v>1020</v>
+        <v>1004</v>
       </c>
       <c r="B7" s="63" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="C7" s="65" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D7" s="63" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E7" s="66">
-        <v>40617</v>
+        <v>40999</v>
       </c>
       <c r="F7" s="74">
-        <v>139</v>
+        <v>10594</v>
       </c>
       <c r="G7" s="66">
-        <v>40983</v>
+        <v>40999</v>
       </c>
       <c r="H7" s="67" t="str">
         <f>"Renewal of Domain and Hosting until "&amp;TEXT(G7,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 15-Mar-2012</v>
+        <v>Renewal of Domain and Hosting until 31-Mar-2012</v>
       </c>
       <c r="I7" s="67" t="str">
         <f>"Renewal of Domain "&amp;B7&amp;" until "&amp;TEXT(G7,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain airylea.com until 15-Mar-2012</v>
+        <v>Renewal of Domain filtra.co.uk until 31-Mar-2012</v>
       </c>
       <c r="J7" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="K7" s="59"/>
+      <c r="K7" s="63" t="s">
+        <v>110</v>
+      </c>
       <c r="L7" s="63" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="M7" s="63" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="N7" s="63" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="O7" s="63" t="s">
-        <v>95</v>
+        <v>93</v>
+      </c>
+      <c r="P7" s="63" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q7" s="63" t="s">
+        <v>99</v>
+      </c>
+      <c r="R7" s="63">
+        <v>3528228</v>
+      </c>
+      <c r="S7" s="80" t="s">
+        <v>113</v>
+      </c>
+      <c r="T7" s="80" t="s">
+        <v>115</v>
+      </c>
+      <c r="U7" s="72">
+        <v>38982</v>
+      </c>
+      <c r="V7" s="72">
+        <v>38989</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="64">
-        <v>1020</v>
+        <v>1004</v>
       </c>
       <c r="B8" s="63" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C8" s="65" t="s">
         <v>66</v>
       </c>
       <c r="D8" s="63" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E8" s="66">
-        <v>40620</v>
+        <v>41018</v>
       </c>
       <c r="F8" s="74">
-        <v>139</v>
+        <v>10595</v>
       </c>
       <c r="G8" s="66">
-        <v>40983</v>
+        <v>40999</v>
       </c>
       <c r="H8" s="67" t="str">
         <f>"Renewal of Domain and Hosting until "&amp;TEXT(G8,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 15-Mar-2012</v>
+        <v>Renewal of Domain and Hosting until 31-Mar-2012</v>
       </c>
       <c r="I8" s="67" t="str">
         <f>"Renewal of Domain "&amp;B8&amp;" until "&amp;TEXT(G8,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain airyleamotors.com until 15-Mar-2012</v>
+        <v>Renewal of Domain midwestmarketforce.co.uk until 31-Mar-2012</v>
       </c>
       <c r="J8" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="K8" s="59"/>
+      <c r="K8" s="81" t="s">
+        <v>106</v>
+      </c>
       <c r="L8" s="63" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="M8" s="63" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="N8" s="63" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="O8" s="63" t="s">
-        <v>95</v>
+        <v>93</v>
+      </c>
+      <c r="P8" s="63" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q8" s="63" t="s">
+        <v>99</v>
+      </c>
+      <c r="R8" s="63">
+        <v>3528228</v>
+      </c>
+      <c r="S8" s="80" t="s">
+        <v>113</v>
+      </c>
+      <c r="T8" s="80" t="s">
+        <v>115</v>
+      </c>
+      <c r="U8" s="72">
+        <v>38982</v>
+      </c>
+      <c r="V8" s="72">
+        <v>38989</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="64">
-        <v>1020</v>
-      </c>
-      <c r="B9" s="63" t="s">
-        <v>122</v>
-      </c>
-      <c r="C9" s="65" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" s="63" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="67">
-        <v>40894</v>
-      </c>
-      <c r="F9" s="79">
-        <v>10329</v>
-      </c>
-      <c r="G9" s="66">
-        <v>40983</v>
+      <c r="A9" s="86">
+        <v>1029</v>
+      </c>
+      <c r="B9" s="87" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9" s="88" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="87" t="s">
+        <v>141</v>
+      </c>
+      <c r="E9" s="89">
+        <v>41008</v>
+      </c>
+      <c r="F9" s="90"/>
+      <c r="G9" s="89">
+        <v>41008</v>
       </c>
       <c r="H9" s="67" t="str">
         <f>"Renewal of Domain and Hosting until "&amp;TEXT(G9,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 15-Mar-2012</v>
-      </c>
-      <c r="I9" s="67" t="str">
+        <v>Renewal of Domain and Hosting until 09-Apr-2012</v>
+      </c>
+      <c r="I9" s="83" t="str">
         <f>"Renewal of Domain "&amp;B9&amp;" until "&amp;TEXT(G9,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain airylea.co.uk until 15-Mar-2012</v>
-      </c>
-      <c r="J9" s="68" t="s">
-        <v>40</v>
-      </c>
-      <c r="K9" s="59"/>
-      <c r="L9" s="63" t="s">
-        <v>46</v>
-      </c>
-      <c r="M9" s="63" t="s">
-        <v>75</v>
-      </c>
-      <c r="N9" s="63" t="s">
-        <v>94</v>
-      </c>
-      <c r="O9" s="63" t="s">
-        <v>95</v>
+        <v>Renewal of Domain jmitchellandson.co.uk until 09-Apr-2012</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="64">
-        <v>1007</v>
+        <v>1002</v>
       </c>
       <c r="B10" s="63" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="C10" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="63" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="76">
-        <v>40992</v>
-      </c>
-      <c r="F10" s="80">
-        <v>140</v>
-      </c>
-      <c r="G10" s="76">
-        <v>40992</v>
+      <c r="D10" s="64" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="66">
+        <v>41034</v>
+      </c>
+      <c r="F10" s="91">
+        <v>135</v>
+      </c>
+      <c r="G10" s="66">
+        <v>41034</v>
       </c>
       <c r="H10" s="67" t="str">
         <f>"Renewal of Domain and Hosting until "&amp;TEXT(G10,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 24-Mar-2012</v>
+        <v>Renewal of Domain and Hosting until 05-May-2012</v>
       </c>
       <c r="I10" s="67" t="str">
         <f>"Renewal of Domain "&amp;B10&amp;" until "&amp;TEXT(G10,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain dsglasscraft.com until 24-Mar-2012</v>
+        <v>Renewal of Domain asrc.biz until 05-May-2012</v>
       </c>
       <c r="J10" s="68" t="s">
         <v>40</v>
       </c>
       <c r="K10" s="59"/>
       <c r="L10" s="63" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="M10" s="63" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="N10" s="63" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="O10" s="63" t="s">
         <v>95</v>
@@ -1668,279 +1727,185 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="64">
-        <v>1004</v>
-      </c>
-      <c r="B11" s="63" t="s">
-        <v>35</v>
+        <v>1031</v>
+      </c>
+      <c r="B11" s="85" t="s">
+        <v>143</v>
       </c>
       <c r="C11" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="63" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="67">
-        <v>41096</v>
-      </c>
-      <c r="F11" s="74">
-        <v>141</v>
+      <c r="D11" s="85" t="s">
+        <v>143</v>
+      </c>
+      <c r="E11" s="66">
+        <v>41076</v>
+      </c>
+      <c r="F11" s="91">
+        <v>142</v>
       </c>
       <c r="G11" s="66">
-        <v>40999</v>
+        <v>41076</v>
       </c>
       <c r="H11" s="67" t="str">
         <f>"Renewal of Domain and Hosting until "&amp;TEXT(G11,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 31-Mar-2012</v>
+        <v>Renewal of Domain and Hosting until 16-Jun-2012</v>
       </c>
       <c r="I11" s="67" t="str">
         <f>"Renewal of Domain "&amp;B11&amp;" until "&amp;TEXT(G11,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain midwestmarketforce.com until 31-Mar-2012</v>
-      </c>
-      <c r="J11" s="68" t="s">
-        <v>40</v>
-      </c>
-      <c r="K11" s="59"/>
-      <c r="L11" s="63" t="s">
-        <v>54</v>
-      </c>
-      <c r="M11" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="N11" s="63" t="s">
-        <v>94</v>
-      </c>
-      <c r="O11" s="63" t="s">
-        <v>95</v>
+        <v>Renewal of Domain loviesdrapery.co.uk  until 16-Jun-2012</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="64">
-        <v>1004</v>
+        <v>1032</v>
       </c>
       <c r="B12" s="63" t="s">
-        <v>33</v>
+        <v>142</v>
       </c>
       <c r="C12" s="65" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D12" s="63" t="s">
-        <v>13</v>
+        <v>142</v>
       </c>
       <c r="E12" s="66">
-        <v>41116</v>
-      </c>
-      <c r="F12" s="74">
-        <v>141</v>
+        <v>41076</v>
+      </c>
+      <c r="F12" s="91">
+        <v>136</v>
       </c>
       <c r="G12" s="66">
-        <v>40999</v>
+        <v>41076</v>
       </c>
       <c r="H12" s="67" t="str">
         <f>"Renewal of Domain and Hosting until "&amp;TEXT(G12,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 31-Mar-2012</v>
+        <v>Renewal of Domain and Hosting until 16-Jun-2012</v>
       </c>
       <c r="I12" s="67" t="str">
         <f>"Renewal of Domain "&amp;B12&amp;" until "&amp;TEXT(G12,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain midwestmarketforce.info until 31-Mar-2012</v>
-      </c>
-      <c r="J12" s="68" t="s">
-        <v>40</v>
-      </c>
-      <c r="K12" s="59"/>
-      <c r="L12" s="63" t="s">
-        <v>54</v>
-      </c>
-      <c r="M12" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="N12" s="63" t="s">
-        <v>101</v>
-      </c>
-      <c r="O12" s="63" t="s">
-        <v>95</v>
+        <v>Renewal of Domain iknit.biz until 16-Jun-2012</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="64">
-        <v>1004</v>
+        <v>1021</v>
       </c>
       <c r="B13" s="63" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C13" s="65" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D13" s="63" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="75">
-        <v>41165</v>
-      </c>
-      <c r="F13" s="74">
-        <v>10593</v>
-      </c>
-      <c r="G13" s="66">
-        <v>40999</v>
+        <v>10</v>
+      </c>
+      <c r="E13" s="67">
+        <v>41116</v>
+      </c>
+      <c r="F13" s="84">
+        <v>20114</v>
+      </c>
+      <c r="G13" s="67">
+        <v>41116</v>
       </c>
       <c r="H13" s="67" t="str">
         <f>"Renewal of Domain and Hosting until "&amp;TEXT(G13,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 31-Mar-2012</v>
+        <v>Renewal of Domain and Hosting until 26-Jul-2012</v>
       </c>
       <c r="I13" s="67" t="str">
         <f>"Renewal of Domain "&amp;B13&amp;" until "&amp;TEXT(G13,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain mwmf.co.uk until 31-Mar-2012</v>
+        <v>Renewal of Domain keptiebakery.com until 26-Jul-2012</v>
       </c>
       <c r="J13" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="K13" s="63" t="s">
-        <v>116</v>
-      </c>
+      <c r="K13" s="59"/>
       <c r="L13" s="63" t="s">
-        <v>54</v>
-      </c>
-      <c r="M13" s="63" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="N13" s="63" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="O13" s="63" t="s">
-        <v>93</v>
-      </c>
-      <c r="P13" s="63" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q13" s="63" t="s">
-        <v>99</v>
-      </c>
-      <c r="R13" s="63">
-        <v>3528228</v>
-      </c>
-      <c r="S13" s="81" t="s">
-        <v>113</v>
-      </c>
-      <c r="T13" s="81" t="s">
-        <v>115</v>
-      </c>
-      <c r="U13" s="72">
-        <v>38982</v>
-      </c>
-      <c r="V13" s="72">
-        <v>38989</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="64">
-        <v>1004</v>
+        <v>1015</v>
       </c>
       <c r="B14" s="63" t="s">
-        <v>31</v>
+        <v>137</v>
       </c>
       <c r="C14" s="65" t="s">
         <v>66</v>
       </c>
       <c r="D14" s="63" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="66">
-        <v>40999</v>
-      </c>
-      <c r="F14" s="74">
-        <v>10594</v>
-      </c>
-      <c r="G14" s="66">
-        <v>40999</v>
+        <v>20</v>
+      </c>
+      <c r="E14" s="75">
+        <v>40860</v>
+      </c>
+      <c r="F14" s="84">
+        <v>20113</v>
+      </c>
+      <c r="G14" s="70">
+        <v>41118</v>
       </c>
       <c r="H14" s="67" t="str">
         <f>"Renewal of Domain and Hosting until "&amp;TEXT(G14,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 31-Mar-2012</v>
+        <v>Renewal of Domain and Hosting until 28-Jul-2012</v>
       </c>
       <c r="I14" s="67" t="str">
         <f>"Renewal of Domain "&amp;B14&amp;" until "&amp;TEXT(G14,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain filtra.co.uk until 31-Mar-2012</v>
+        <v>Renewal of Domain stourvalleytechnicalservices.co.uk until 28-Jul-2012</v>
       </c>
       <c r="J14" s="68" t="s">
         <v>40</v>
-      </c>
-      <c r="K14" s="63" t="s">
-        <v>110</v>
-      </c>
-      <c r="L14" s="63" t="s">
-        <v>54</v>
-      </c>
-      <c r="M14" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="N14" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="O14" s="63" t="s">
-        <v>93</v>
-      </c>
-      <c r="P14" s="63" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q14" s="63" t="s">
-        <v>99</v>
-      </c>
-      <c r="R14" s="63">
-        <v>3528228</v>
-      </c>
-      <c r="S14" s="81" t="s">
-        <v>113</v>
-      </c>
-      <c r="T14" s="81" t="s">
-        <v>115</v>
-      </c>
-      <c r="U14" s="72">
-        <v>38982</v>
-      </c>
-      <c r="V14" s="72">
-        <v>38989</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="64">
-        <v>1004</v>
+        <v>1015</v>
       </c>
       <c r="B15" s="63" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="C15" s="65" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D15" s="63" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="66">
-        <v>41018</v>
-      </c>
-      <c r="F15" s="74">
-        <v>10595</v>
-      </c>
-      <c r="G15" s="66">
-        <v>40999</v>
+        <v>20</v>
+      </c>
+      <c r="E15" s="70">
+        <v>41483</v>
+      </c>
+      <c r="F15" s="91">
+        <v>137</v>
+      </c>
+      <c r="G15" s="70">
+        <v>41118</v>
       </c>
       <c r="H15" s="67" t="str">
         <f>"Renewal of Domain and Hosting until "&amp;TEXT(G15,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 31-Mar-2012</v>
+        <v>Renewal of Domain and Hosting until 28-Jul-2012</v>
       </c>
       <c r="I15" s="67" t="str">
         <f>"Renewal of Domain "&amp;B15&amp;" until "&amp;TEXT(G15,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain midwestmarketforce.co.uk until 31-Mar-2012</v>
+        <v>Renewal of Domain stourvalleytimberengineering.co.uk until 28-Jul-2012</v>
       </c>
       <c r="J15" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="K15" s="82" t="s">
-        <v>106</v>
+      <c r="K15" s="63" t="s">
+        <v>118</v>
       </c>
       <c r="L15" s="63" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="M15" s="63" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="N15" s="63" t="s">
         <v>92</v>
@@ -1949,391 +1914,418 @@
         <v>93</v>
       </c>
       <c r="P15" s="63" t="s">
-        <v>98</v>
+        <v>49</v>
       </c>
       <c r="Q15" s="63" t="s">
-        <v>99</v>
-      </c>
-      <c r="R15" s="63">
-        <v>3528228</v>
-      </c>
-      <c r="S15" s="81" t="s">
-        <v>113</v>
-      </c>
-      <c r="T15" s="81" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="U15" s="72">
-        <v>38982</v>
+        <v>38985</v>
       </c>
       <c r="V15" s="72">
         <v>38989</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="87">
-        <v>1029</v>
-      </c>
-      <c r="B16" s="88" t="s">
-        <v>141</v>
-      </c>
-      <c r="C16" s="89" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="88" t="s">
-        <v>141</v>
-      </c>
-      <c r="E16" s="90">
-        <v>41008</v>
-      </c>
-      <c r="F16" s="91"/>
-      <c r="G16" s="90">
-        <v>41008</v>
+      <c r="A16" s="64">
+        <v>1015</v>
+      </c>
+      <c r="B16" s="63" t="s">
+        <v>138</v>
+      </c>
+      <c r="C16" s="65" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="63" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="75">
+        <v>40619</v>
+      </c>
+      <c r="F16" s="91">
+        <v>137</v>
+      </c>
+      <c r="G16" s="70">
+        <v>41118</v>
       </c>
       <c r="H16" s="67" t="str">
         <f>"Renewal of Domain and Hosting until "&amp;TEXT(G16,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 09-Apr-2012</v>
-      </c>
-      <c r="I16" s="84" t="str">
+        <v>Renewal of Domain and Hosting until 28-Jul-2012</v>
+      </c>
+      <c r="I16" s="67" t="str">
         <f>"Renewal of Domain "&amp;B16&amp;" until "&amp;TEXT(G16,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain jmitchellandson.co.uk until 09-Apr-2012</v>
+        <v>Renewal of Domain svts.co.uk until 28-Jul-2012</v>
+      </c>
+      <c r="J16" s="68" t="s">
+        <v>40</v>
+      </c>
+      <c r="L16" s="63" t="s">
+        <v>60</v>
+      </c>
+      <c r="M16" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="N16" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="O16" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="P16" s="63" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="64">
-        <v>1002</v>
+        <v>1015</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>67</v>
+        <v>125</v>
       </c>
       <c r="C17" s="65" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="64" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" s="66">
-        <v>41034</v>
-      </c>
-      <c r="F17" s="92">
-        <v>135</v>
-      </c>
-      <c r="G17" s="66">
-        <v>41034</v>
+        <v>66</v>
+      </c>
+      <c r="D17" s="63" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="75">
+        <v>40821</v>
+      </c>
+      <c r="F17" s="91">
+        <v>137</v>
+      </c>
+      <c r="G17" s="70">
+        <v>41118</v>
       </c>
       <c r="H17" s="67" t="str">
         <f>"Renewal of Domain and Hosting until "&amp;TEXT(G17,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 05-May-2012</v>
+        <v>Renewal of Domain and Hosting until 28-Jul-2012</v>
       </c>
       <c r="I17" s="67" t="str">
         <f>"Renewal of Domain "&amp;B17&amp;" until "&amp;TEXT(G17,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain asrc.biz until 05-May-2012</v>
+        <v>Renewal of Domain svte.co.uk until 28-Jul-2012</v>
       </c>
       <c r="J17" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="K17" s="59"/>
       <c r="L17" s="63" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="M17" s="63" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="N17" s="63" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="O17" s="63" t="s">
-        <v>95</v>
+        <v>93</v>
+      </c>
+      <c r="P17" s="63" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="64">
-        <v>1031</v>
-      </c>
-      <c r="B18" s="86" t="s">
-        <v>143</v>
+        <v>1016</v>
+      </c>
+      <c r="B18" s="63" t="s">
+        <v>21</v>
       </c>
       <c r="C18" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="86" t="s">
-        <v>143</v>
-      </c>
-      <c r="E18" s="66">
-        <v>41076</v>
-      </c>
-      <c r="F18" s="92">
-        <v>142</v>
-      </c>
-      <c r="G18" s="66">
-        <v>41076</v>
+      <c r="D18" s="63" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="75">
+        <v>40791</v>
+      </c>
+      <c r="F18" s="84">
+        <v>156</v>
+      </c>
+      <c r="G18" s="75">
+        <v>41157</v>
       </c>
       <c r="H18" s="67" t="str">
         <f>"Renewal of Domain and Hosting until "&amp;TEXT(G18,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 16-Jun-2012</v>
+        <v>Renewal of Domain and Hosting until 05-Sep-2012</v>
       </c>
       <c r="I18" s="67" t="str">
         <f>"Renewal of Domain "&amp;B18&amp;" until "&amp;TEXT(G18,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain loviesdrapery.co.uk  until 16-Jun-2012</v>
+        <v>Renewal of Domain walterpatterson.net until 05-Sep-2012</v>
+      </c>
+      <c r="J18" s="68" t="s">
+        <v>40</v>
+      </c>
+      <c r="K18" s="59"/>
+      <c r="L18" s="63" t="s">
+        <v>56</v>
+      </c>
+      <c r="M18" s="63" t="s">
+        <v>81</v>
+      </c>
+      <c r="N18" s="63" t="s">
+        <v>102</v>
+      </c>
+      <c r="O18" s="63" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="64">
-        <v>1032</v>
+        <v>1028</v>
       </c>
       <c r="B19" s="63" t="s">
-        <v>142</v>
+        <v>12</v>
       </c>
       <c r="C19" s="65" t="s">
         <v>65</v>
       </c>
       <c r="D19" s="63" t="s">
-        <v>142</v>
-      </c>
-      <c r="E19" s="66">
-        <v>41076</v>
-      </c>
-      <c r="F19" s="92">
-        <v>136</v>
-      </c>
-      <c r="G19" s="66">
-        <v>41076</v>
+        <v>12</v>
+      </c>
+      <c r="E19" s="70">
+        <v>41195</v>
+      </c>
+      <c r="F19" s="84">
+        <v>20122</v>
+      </c>
+      <c r="G19" s="70">
+        <v>41195</v>
       </c>
       <c r="H19" s="67" t="str">
         <f>"Renewal of Domain and Hosting until "&amp;TEXT(G19,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 16-Jun-2012</v>
+        <v>Renewal of Domain and Hosting until 13-Oct-2012</v>
       </c>
       <c r="I19" s="67" t="str">
         <f>"Renewal of Domain "&amp;B19&amp;" until "&amp;TEXT(G19,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain iknit.biz until 16-Jun-2012</v>
+        <v>Renewal of Domain mapleleafcards.com until 13-Oct-2012</v>
+      </c>
+      <c r="J19" s="68" t="s">
+        <v>40</v>
+      </c>
+      <c r="K19" s="59"/>
+      <c r="L19" s="63" t="s">
+        <v>53</v>
+      </c>
+      <c r="N19" s="63" t="s">
+        <v>94</v>
+      </c>
+      <c r="O19" s="63" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="64">
-        <v>1021</v>
-      </c>
       <c r="B20" s="63" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="C20" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="63" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="67">
-        <v>41116</v>
-      </c>
-      <c r="F20" s="85">
-        <v>20114</v>
-      </c>
-      <c r="G20" s="67">
-        <v>41116</v>
+      <c r="D20" s="64" t="s">
+        <v>136</v>
+      </c>
+      <c r="E20" s="75">
+        <v>41223</v>
+      </c>
+      <c r="G20" s="75">
+        <v>41223</v>
       </c>
       <c r="H20" s="67" t="str">
         <f>"Renewal of Domain and Hosting until "&amp;TEXT(G20,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 26-Jul-2012</v>
+        <v>Renewal of Domain and Hosting until 10-Nov-2012</v>
       </c>
       <c r="I20" s="67" t="str">
         <f>"Renewal of Domain "&amp;B20&amp;" until "&amp;TEXT(G20,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain keptiebakery.com until 26-Jul-2012</v>
+        <v>Renewal of Domain goodteaching.org until 10-Nov-2012</v>
       </c>
       <c r="J20" s="68" t="s">
         <v>40</v>
-      </c>
-      <c r="K20" s="59"/>
-      <c r="L20" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="N20" s="63" t="s">
-        <v>94</v>
-      </c>
-      <c r="O20" s="63" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="64">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="B21" s="63" t="s">
-        <v>137</v>
+        <v>16</v>
       </c>
       <c r="C21" s="65" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D21" s="63" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E21" s="75">
-        <v>40860</v>
-      </c>
-      <c r="F21" s="85">
-        <v>20113</v>
-      </c>
-      <c r="G21" s="70">
-        <v>41118</v>
+        <v>41223</v>
+      </c>
+      <c r="F21" s="71">
+        <v>10309</v>
+      </c>
+      <c r="G21" s="75">
+        <v>41223</v>
       </c>
       <c r="H21" s="67" t="str">
         <f>"Renewal of Domain and Hosting until "&amp;TEXT(G21,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 28-Jul-2012</v>
+        <v>Renewal of Domain and Hosting until 10-Nov-2012</v>
       </c>
       <c r="I21" s="67" t="str">
         <f>"Renewal of Domain "&amp;B21&amp;" until "&amp;TEXT(G21,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain stourvalleytechnicalservices.co.uk until 28-Jul-2012</v>
+        <v>Renewal of Domain powersoftware.com until 10-Nov-2012</v>
       </c>
       <c r="J21" s="68" t="s">
         <v>40</v>
+      </c>
+      <c r="K21" s="59"/>
+      <c r="L21" s="63" t="s">
+        <v>57</v>
+      </c>
+      <c r="M21" s="63" t="s">
+        <v>83</v>
+      </c>
+      <c r="N21" s="63" t="s">
+        <v>94</v>
+      </c>
+      <c r="O21" s="63" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="64">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="B22" s="63" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C22" s="65" t="s">
         <v>65</v>
       </c>
       <c r="D22" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="70">
-        <v>41483</v>
-      </c>
-      <c r="F22" s="92">
-        <v>137</v>
-      </c>
-      <c r="G22" s="70">
-        <v>41118</v>
+        <v>22</v>
+      </c>
+      <c r="E22" s="66">
+        <v>41223</v>
+      </c>
+      <c r="F22" s="84">
+        <v>20124</v>
+      </c>
+      <c r="G22" s="66">
+        <v>41223</v>
       </c>
       <c r="H22" s="67" t="str">
         <f>"Renewal of Domain and Hosting until "&amp;TEXT(G22,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 28-Jul-2012</v>
+        <v>Renewal of Domain and Hosting until 10-Nov-2012</v>
       </c>
       <c r="I22" s="67" t="str">
         <f>"Renewal of Domain "&amp;B22&amp;" until "&amp;TEXT(G22,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain stourvalleytimberengineering.co.uk until 28-Jul-2012</v>
+        <v>Renewal of Domain westcoastexpress.net until 10-Nov-2012</v>
       </c>
       <c r="J22" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="K22" s="63" t="s">
-        <v>118</v>
-      </c>
+      <c r="K22" s="59"/>
       <c r="L22" s="63" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="M22" s="63" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="N22" s="63" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="O22" s="63" t="s">
-        <v>93</v>
-      </c>
-      <c r="P22" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q22" s="63" t="s">
-        <v>97</v>
-      </c>
-      <c r="U22" s="72">
-        <v>38985</v>
-      </c>
-      <c r="V22" s="72">
-        <v>38989</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="P22" s="77"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="64">
-        <v>1015</v>
+        <v>1001</v>
       </c>
       <c r="B23" s="63" t="s">
-        <v>138</v>
+        <v>17</v>
       </c>
       <c r="C23" s="65" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D23" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" s="75">
-        <v>40619</v>
-      </c>
-      <c r="F23" s="92">
-        <v>137</v>
-      </c>
-      <c r="G23" s="70">
-        <v>41118</v>
+        <v>17</v>
+      </c>
+      <c r="E23" s="76">
+        <v>40965</v>
+      </c>
+      <c r="F23" s="74">
+        <v>188</v>
+      </c>
+      <c r="G23" s="76">
+        <v>41331</v>
       </c>
       <c r="H23" s="67" t="str">
         <f>"Renewal of Domain and Hosting until "&amp;TEXT(G23,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 28-Jul-2012</v>
+        <v>Renewal of Domain and Hosting until 26-Feb-2013</v>
       </c>
       <c r="I23" s="67" t="str">
         <f>"Renewal of Domain "&amp;B23&amp;" until "&amp;TEXT(G23,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain svts.co.uk until 28-Jul-2012</v>
+        <v>Renewal of Domain relaxatub.com until 26-Feb-2013</v>
       </c>
       <c r="J23" s="68" t="s">
         <v>40</v>
       </c>
+      <c r="K23" s="59"/>
       <c r="L23" s="63" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="M23" s="63" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="N23" s="63" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="O23" s="63" t="s">
-        <v>93</v>
-      </c>
-      <c r="P23" s="63" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="64">
-        <v>1015</v>
+        <v>1001</v>
       </c>
       <c r="B24" s="63" t="s">
-        <v>125</v>
+        <v>37</v>
       </c>
       <c r="C24" s="65" t="s">
         <v>66</v>
       </c>
       <c r="D24" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" s="75">
-        <v>40821</v>
-      </c>
-      <c r="F24" s="92">
-        <v>137</v>
-      </c>
-      <c r="G24" s="70">
-        <v>41118</v>
+        <v>17</v>
+      </c>
+      <c r="E24" s="76">
+        <v>41331</v>
+      </c>
+      <c r="F24" s="74">
+        <v>138</v>
+      </c>
+      <c r="G24" s="76">
+        <v>41331</v>
       </c>
       <c r="H24" s="67" t="str">
         <f>"Renewal of Domain and Hosting until "&amp;TEXT(G24,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 28-Jul-2012</v>
+        <v>Renewal of Domain and Hosting until 26-Feb-2013</v>
       </c>
       <c r="I24" s="67" t="str">
         <f>"Renewal of Domain "&amp;B24&amp;" until "&amp;TEXT(G24,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain svte.co.uk until 28-Jul-2012</v>
+        <v>Renewal of Domain relaxatub.co.uk until 26-Feb-2013</v>
       </c>
       <c r="J24" s="68" t="s">
         <v>40</v>
       </c>
+      <c r="K24" s="63" t="s">
+        <v>107</v>
+      </c>
       <c r="L24" s="63" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="M24" s="63" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="N24" s="63" t="s">
         <v>92</v>
@@ -2342,51 +2334,60 @@
         <v>93</v>
       </c>
       <c r="P24" s="63" t="s">
-        <v>60</v>
+        <v>103</v>
+      </c>
+      <c r="Q24" s="63" t="s">
+        <v>97</v>
+      </c>
+      <c r="U24" s="72">
+        <v>38982</v>
+      </c>
+      <c r="V24" s="72">
+        <v>38989</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="64">
-        <v>1016</v>
+        <v>1020</v>
       </c>
       <c r="B25" s="63" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C25" s="65" t="s">
         <v>65</v>
       </c>
       <c r="D25" s="63" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" s="75">
-        <v>40791</v>
-      </c>
-      <c r="F25" s="85">
-        <v>156</v>
-      </c>
-      <c r="G25" s="75">
-        <v>41157</v>
+        <v>3</v>
+      </c>
+      <c r="E25" s="66">
+        <v>41348</v>
+      </c>
+      <c r="F25" s="74">
+        <v>189</v>
+      </c>
+      <c r="G25" s="66">
+        <v>41348</v>
       </c>
       <c r="H25" s="67" t="str">
         <f>"Renewal of Domain and Hosting until "&amp;TEXT(G25,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 05-Sep-2012</v>
+        <v>Renewal of Domain and Hosting until 15-Mar-2013</v>
       </c>
       <c r="I25" s="67" t="str">
         <f>"Renewal of Domain "&amp;B25&amp;" until "&amp;TEXT(G25,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain walterpatterson.net until 05-Sep-2012</v>
+        <v>Renewal of Domain airylea.com until 15-Mar-2013</v>
       </c>
       <c r="J25" s="68" t="s">
         <v>40</v>
       </c>
       <c r="K25" s="59"/>
       <c r="L25" s="63" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="M25" s="63" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="N25" s="63" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="O25" s="63" t="s">
         <v>95</v>
@@ -2394,40 +2395,43 @@
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="64">
-        <v>1028</v>
+        <v>1020</v>
       </c>
       <c r="B26" s="63" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C26" s="65" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D26" s="63" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="70">
-        <v>41195</v>
-      </c>
-      <c r="F26" s="85">
-        <v>20122</v>
-      </c>
-      <c r="G26" s="70">
-        <v>41195</v>
+        <v>3</v>
+      </c>
+      <c r="E26" s="66">
+        <v>41351</v>
+      </c>
+      <c r="F26" s="74">
+        <v>189</v>
+      </c>
+      <c r="G26" s="66">
+        <v>41348</v>
       </c>
       <c r="H26" s="67" t="str">
         <f>"Renewal of Domain and Hosting until "&amp;TEXT(G26,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 13-Oct-2012</v>
+        <v>Renewal of Domain and Hosting until 15-Mar-2013</v>
       </c>
       <c r="I26" s="67" t="str">
         <f>"Renewal of Domain "&amp;B26&amp;" until "&amp;TEXT(G26,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain mapleleafcards.com until 13-Oct-2012</v>
+        <v>Renewal of Domain airyleamotors.com until 15-Mar-2013</v>
       </c>
       <c r="J26" s="68" t="s">
         <v>40</v>
       </c>
       <c r="K26" s="59"/>
       <c r="L26" s="63" t="s">
-        <v>53</v>
+        <v>46</v>
+      </c>
+      <c r="M26" s="63" t="s">
+        <v>75</v>
       </c>
       <c r="N26" s="63" t="s">
         <v>94</v>
@@ -2438,63 +2442,49 @@
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="64">
-        <v>1001</v>
+        <v>1020</v>
       </c>
       <c r="B27" s="63" t="s">
-        <v>37</v>
+        <v>122</v>
       </c>
       <c r="C27" s="65" t="s">
         <v>66</v>
       </c>
       <c r="D27" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="E27" s="76">
-        <v>41331</v>
+        <v>3</v>
+      </c>
+      <c r="E27" s="67">
+        <v>41625</v>
       </c>
       <c r="F27" s="74">
-        <v>138</v>
-      </c>
-      <c r="G27" s="76">
-        <v>41331</v>
+        <v>189</v>
+      </c>
+      <c r="G27" s="66">
+        <v>41713</v>
       </c>
       <c r="H27" s="67" t="str">
         <f>"Renewal of Domain and Hosting until "&amp;TEXT(G27,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 26-Feb-2013</v>
+        <v>Renewal of Domain and Hosting until 15-Mar-2014</v>
       </c>
       <c r="I27" s="67" t="str">
         <f>"Renewal of Domain "&amp;B27&amp;" until "&amp;TEXT(G27,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain relaxatub.co.uk until 26-Feb-2013</v>
+        <v>Renewal of Domain airylea.co.uk until 15-Mar-2014</v>
       </c>
       <c r="J27" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="K27" s="63" t="s">
-        <v>107</v>
-      </c>
+      <c r="K27" s="59"/>
       <c r="L27" s="63" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="M27" s="63" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="N27" s="63" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="O27" s="63" t="s">
-        <v>93</v>
-      </c>
-      <c r="P27" s="63" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q27" s="63" t="s">
-        <v>97</v>
-      </c>
-      <c r="U27" s="72">
-        <v>38982</v>
-      </c>
-      <c r="V27" s="72">
-        <v>38989</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
@@ -3715,7 +3705,7 @@
       <c r="E21" s="73">
         <v>40791</v>
       </c>
-      <c r="F21" s="85">
+      <c r="F21" s="84">
         <v>20116</v>
       </c>
       <c r="G21" s="73">
@@ -3776,7 +3766,7 @@
       <c r="E22" s="76">
         <v>40855</v>
       </c>
-      <c r="F22" s="85">
+      <c r="F22" s="84">
         <v>20120</v>
       </c>
       <c r="G22" s="76">

</xml_diff>

<commit_message>
Domains updated for invoice run.
</commit_message>
<xml_diff>
--- a/clients/Domains.xlsx
+++ b/clients/Domains.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="15600" windowHeight="11670"/>
+    <workbookView xWindow="483" yWindow="121" windowWidth="15599" windowHeight="11671"/>
   </bookViews>
   <sheets>
     <sheet name="Domains" sheetId="2" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="NoLongerManaged" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Domains!$A$1:$L$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Domains!$A$1:$L$23</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -650,7 +650,7 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -826,9 +826,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="13" fillId="11" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1154,42 +1151,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V31"/>
+  <dimension ref="A1:V27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="64" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" style="63" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="65" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.5703125" style="65" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="81" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="74" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.73046875" style="64" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.59765625" style="63" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.265625" style="65" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.59765625" style="65" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1328125" style="81" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.3984375" style="74" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" style="74" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="46.5703125" style="74" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="67.42578125" style="74" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.28515625" style="63" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" style="63" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.42578125" style="63" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" style="63" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.140625" style="63" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46.59765625" style="74" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="67.3984375" style="74" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.265625" style="63" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.1328125" style="63" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.3984375" style="63" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.3984375" style="63" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.1328125" style="63" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8" style="63" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.42578125" style="63" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="57.85546875" style="63" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" style="63" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="15.42578125" style="63" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="24.140625" style="63" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.7109375" style="63" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="63"/>
+    <col min="16" max="16" width="24.3984375" style="63" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="57.86328125" style="63" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.86328125" style="63" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="15.3984375" style="63" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24.1328125" style="63" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.73046875" style="63" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.1328125" style="63"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A1" s="58" t="s">
         <v>23</v>
       </c>
@@ -1254,311 +1251,287 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="85">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A2" s="84">
         <v>1029</v>
       </c>
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="85" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="87" t="s">
+      <c r="C2" s="86" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="86" t="s">
+      <c r="D2" s="85" t="s">
         <v>141</v>
       </c>
-      <c r="E2" s="88">
+      <c r="E2" s="87">
         <v>41008</v>
       </c>
-      <c r="F2" s="89"/>
-      <c r="G2" s="88">
+      <c r="F2" s="88"/>
+      <c r="G2" s="87">
         <v>41008</v>
       </c>
       <c r="H2" s="67" t="str">
-        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G2,"dd-MMM-yyyy")</f>
+        <f>"Renewal of Domain and Hosting until "&amp;TEXT(E2,"dd-MMM-yyyy")</f>
         <v>Renewal of Domain and Hosting until 09-Apr-2012</v>
       </c>
-      <c r="I2" s="82" t="str">
-        <f>"Renewal of Domain "&amp;B2&amp;" until "&amp;TEXT(G2,"dd-MMM-yyyy")</f>
+      <c r="I2" s="67" t="str">
+        <f>"Renewal of Domain "&amp;B2&amp;" until "&amp;TEXT(E2,"dd-MMM-yyyy")</f>
         <v>Renewal of Domain jmitchellandson.co.uk until 09-Apr-2012</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A3" s="64">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="B3" s="63" t="s">
-        <v>137</v>
+        <v>21</v>
       </c>
       <c r="C3" s="65" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" s="63" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" s="75">
-        <v>40860</v>
-      </c>
-      <c r="F3" s="83">
-        <v>20113</v>
-      </c>
-      <c r="G3" s="70">
-        <v>41118</v>
+        <v>40791</v>
+      </c>
+      <c r="F3" s="82">
+        <v>156</v>
+      </c>
+      <c r="G3" s="75">
+        <v>41157</v>
       </c>
       <c r="H3" s="67" t="str">
-        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G3,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 28-Jul-2012</v>
+        <f>"Renewal of Domain and Hosting until "&amp;TEXT(E3,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain and Hosting until 05-Sep-2011</v>
       </c>
       <c r="I3" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B3&amp;" until "&amp;TEXT(G3,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain stourvalleytechnicalservices.co.uk until 28-Jul-2012</v>
+        <f>"Renewal of Domain "&amp;B3&amp;" until "&amp;TEXT(E3,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain walterpatterson.net until 05-Sep-2011</v>
       </c>
       <c r="J3" s="68" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="K3" s="59"/>
+      <c r="L3" s="63" t="s">
+        <v>56</v>
+      </c>
+      <c r="M3" s="63" t="s">
+        <v>81</v>
+      </c>
+      <c r="N3" s="63" t="s">
+        <v>102</v>
+      </c>
+      <c r="O3" s="63" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A4" s="64">
-        <v>1015</v>
+        <v>1028</v>
       </c>
       <c r="B4" s="63" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C4" s="65" t="s">
         <v>65</v>
       </c>
       <c r="D4" s="63" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E4" s="70">
-        <v>41483</v>
-      </c>
-      <c r="F4" s="90">
-        <v>137</v>
+        <v>41195</v>
+      </c>
+      <c r="F4" s="82">
+        <v>20122</v>
       </c>
       <c r="G4" s="70">
-        <v>41118</v>
+        <v>41195</v>
       </c>
       <c r="H4" s="67" t="str">
-        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G4,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 28-Jul-2012</v>
+        <f>"Renewal of Domain and Hosting until "&amp;TEXT(E4,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain and Hosting until 13-Oct-2012</v>
       </c>
       <c r="I4" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B4&amp;" until "&amp;TEXT(G4,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain stourvalleytimberengineering.co.uk until 28-Jul-2012</v>
+        <f>"Renewal of Domain "&amp;B4&amp;" until "&amp;TEXT(E4,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain mapleleafcards.com until 13-Oct-2012</v>
       </c>
       <c r="J4" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="63" t="s">
-        <v>118</v>
-      </c>
+      <c r="K4" s="59"/>
       <c r="L4" s="63" t="s">
-        <v>60</v>
-      </c>
-      <c r="M4" s="63" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="N4" s="63" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="O4" s="63" t="s">
-        <v>93</v>
-      </c>
-      <c r="P4" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q4" s="63" t="s">
-        <v>97</v>
-      </c>
-      <c r="U4" s="72">
-        <v>38985</v>
-      </c>
-      <c r="V4" s="72">
-        <v>38989</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="64">
-        <v>1015</v>
-      </c>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B5" s="63" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C5" s="65" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" s="63" t="s">
-        <v>20</v>
+        <v>65</v>
+      </c>
+      <c r="D5" s="64" t="s">
+        <v>136</v>
       </c>
       <c r="E5" s="75">
-        <v>40619</v>
-      </c>
-      <c r="F5" s="90">
-        <v>137</v>
-      </c>
-      <c r="G5" s="70">
-        <v>41118</v>
+        <v>41223</v>
+      </c>
+      <c r="G5" s="75">
+        <v>41223</v>
       </c>
       <c r="H5" s="67" t="str">
-        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G5,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 28-Jul-2012</v>
+        <f>"Renewal of Domain and Hosting until "&amp;TEXT(E5,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain and Hosting until 10-Nov-2012</v>
       </c>
       <c r="I5" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B5&amp;" until "&amp;TEXT(G5,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain svts.co.uk until 28-Jul-2012</v>
+        <f>"Renewal of Domain "&amp;B5&amp;" until "&amp;TEXT(E5,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain goodteaching.org until 10-Nov-2012</v>
       </c>
       <c r="J5" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="L5" s="63" t="s">
-        <v>60</v>
-      </c>
-      <c r="M5" s="63" t="s">
-        <v>85</v>
-      </c>
-      <c r="N5" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="O5" s="63" t="s">
-        <v>93</v>
-      </c>
-      <c r="P5" s="63" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A6" s="64">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="B6" s="63" t="s">
-        <v>125</v>
+        <v>16</v>
       </c>
       <c r="C6" s="65" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D6" s="63" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E6" s="75">
-        <v>40821</v>
-      </c>
-      <c r="F6" s="90">
-        <v>137</v>
-      </c>
-      <c r="G6" s="70">
-        <v>41118</v>
+        <v>41223</v>
+      </c>
+      <c r="F6" s="71">
+        <v>10309</v>
+      </c>
+      <c r="G6" s="75">
+        <v>41223</v>
       </c>
       <c r="H6" s="67" t="str">
-        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G6,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 28-Jul-2012</v>
+        <f>"Renewal of Domain and Hosting until "&amp;TEXT(E6,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain and Hosting until 10-Nov-2012</v>
       </c>
       <c r="I6" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B6&amp;" until "&amp;TEXT(G6,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain svte.co.uk until 28-Jul-2012</v>
+        <f>"Renewal of Domain "&amp;B6&amp;" until "&amp;TEXT(E6,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain powersoftware.com until 10-Nov-2012</v>
       </c>
       <c r="J6" s="68" t="s">
         <v>40</v>
       </c>
+      <c r="K6" s="59"/>
       <c r="L6" s="63" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M6" s="63" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="N6" s="63" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="O6" s="63" t="s">
-        <v>93</v>
-      </c>
-      <c r="P6" s="63" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A7" s="64">
-        <v>1016</v>
+        <v>1010</v>
       </c>
       <c r="B7" s="63" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C7" s="65" t="s">
         <v>65</v>
       </c>
       <c r="D7" s="63" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="75">
-        <v>40791</v>
-      </c>
-      <c r="F7" s="83">
-        <v>156</v>
-      </c>
-      <c r="G7" s="75">
-        <v>41157</v>
+        <v>14</v>
+      </c>
+      <c r="E7" s="78">
+        <v>41648</v>
+      </c>
+      <c r="F7" s="82">
+        <v>205</v>
+      </c>
+      <c r="G7" s="78">
+        <v>41648</v>
       </c>
       <c r="H7" s="67" t="str">
-        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G7,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 05-Sep-2012</v>
+        <f>"Renewal of Domain and Hosting until "&amp;TEXT(E7,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain and Hosting until 09-Jan-2014</v>
       </c>
       <c r="I7" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B7&amp;" until "&amp;TEXT(G7,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain walterpatterson.net until 05-Sep-2012</v>
+        <f>"Renewal of Domain "&amp;B7&amp;" until "&amp;TEXT(E7,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain onestopaberdeen.com until 09-Jan-2014</v>
       </c>
       <c r="J7" s="68" t="s">
         <v>40</v>
       </c>
       <c r="K7" s="59"/>
       <c r="L7" s="63" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M7" s="63" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N7" s="63" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="O7" s="63" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A8" s="64">
-        <v>1028</v>
+        <v>1007</v>
       </c>
       <c r="B8" s="63" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C8" s="65" t="s">
         <v>65</v>
       </c>
       <c r="D8" s="63" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="70">
-        <v>41195</v>
-      </c>
-      <c r="F8" s="83">
-        <v>20122</v>
-      </c>
-      <c r="G8" s="70">
-        <v>41195</v>
+        <v>5</v>
+      </c>
+      <c r="E8" s="76">
+        <v>41357</v>
+      </c>
+      <c r="F8" s="82">
+        <v>194</v>
+      </c>
+      <c r="G8" s="76">
+        <v>41357</v>
       </c>
       <c r="H8" s="67" t="str">
-        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G8,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 13-Oct-2012</v>
+        <f>"Renewal of Domain and Hosting until "&amp;TEXT(E8,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain and Hosting until 24-Mar-2013</v>
       </c>
       <c r="I8" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B8&amp;" until "&amp;TEXT(G8,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain mapleleafcards.com until 13-Oct-2012</v>
+        <f>"Renewal of Domain "&amp;B8&amp;" until "&amp;TEXT(E8,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain dsglasscraft.com until 24-Mar-2013</v>
       </c>
       <c r="J8" s="68" t="s">
         <v>40</v>
       </c>
       <c r="K8" s="59"/>
       <c r="L8" s="63" t="s">
-        <v>53</v>
+        <v>48</v>
+      </c>
+      <c r="M8" s="63" t="s">
+        <v>76</v>
       </c>
       <c r="N8" s="63" t="s">
         <v>94</v>
@@ -1567,370 +1540,343 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A9" s="64">
+        <v>1004</v>
+      </c>
       <c r="B9" s="63" t="s">
-        <v>136</v>
+        <v>35</v>
       </c>
       <c r="C9" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="64" t="s">
-        <v>136</v>
-      </c>
-      <c r="E9" s="75">
-        <v>41223</v>
-      </c>
-      <c r="G9" s="75">
-        <v>41223</v>
+      <c r="D9" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="67">
+        <v>41461</v>
+      </c>
+      <c r="F9" s="74">
+        <v>191</v>
+      </c>
+      <c r="G9" s="66">
+        <v>41364</v>
       </c>
       <c r="H9" s="67" t="str">
-        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G9,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 10-Nov-2012</v>
+        <f>"Renewal of Domain and Hosting until "&amp;TEXT(E9,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain and Hosting until 06-Jul-2013</v>
       </c>
       <c r="I9" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B9&amp;" until "&amp;TEXT(G9,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain goodteaching.org until 10-Nov-2012</v>
+        <f>"Renewal of Domain "&amp;B9&amp;" until "&amp;TEXT(E9,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain midwestmarketforce.com until 06-Jul-2013</v>
       </c>
       <c r="J9" s="68" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="K9" s="59"/>
+      <c r="L9" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="M9" s="63" t="s">
+        <v>73</v>
+      </c>
+      <c r="N9" s="63" t="s">
+        <v>94</v>
+      </c>
+      <c r="O9" s="63" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A10" s="64">
-        <v>1013</v>
+        <v>1004</v>
       </c>
       <c r="B10" s="63" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C10" s="65" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D10" s="63" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="75">
-        <v>41223</v>
-      </c>
-      <c r="F10" s="71">
-        <v>10309</v>
-      </c>
-      <c r="G10" s="75">
-        <v>41223</v>
+        <v>13</v>
+      </c>
+      <c r="E10" s="66">
+        <v>41481</v>
+      </c>
+      <c r="F10" s="74">
+        <v>191</v>
+      </c>
+      <c r="G10" s="66">
+        <v>41364</v>
       </c>
       <c r="H10" s="67" t="str">
-        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G10,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 10-Nov-2012</v>
+        <f>"Renewal of Domain and Hosting until "&amp;TEXT(E10,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain and Hosting until 26-Jul-2013</v>
       </c>
       <c r="I10" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B10&amp;" until "&amp;TEXT(G10,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain powersoftware.com until 10-Nov-2012</v>
+        <f>"Renewal of Domain "&amp;B10&amp;" until "&amp;TEXT(E10,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain midwestmarketforce.info until 26-Jul-2013</v>
       </c>
       <c r="J10" s="68" t="s">
         <v>40</v>
       </c>
       <c r="K10" s="59"/>
       <c r="L10" s="63" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="M10" s="63" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="N10" s="63" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="O10" s="63" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A11" s="64">
-        <v>1017</v>
+        <v>1032</v>
       </c>
       <c r="B11" s="63" t="s">
-        <v>22</v>
+        <v>144</v>
       </c>
       <c r="C11" s="65" t="s">
         <v>65</v>
       </c>
       <c r="D11" s="63" t="s">
-        <v>22</v>
+        <v>144</v>
       </c>
       <c r="E11" s="66">
-        <v>41223</v>
-      </c>
-      <c r="F11" s="83">
-        <v>20124</v>
+        <v>41383</v>
+      </c>
+      <c r="F11" s="82">
+        <v>193</v>
       </c>
       <c r="G11" s="66">
-        <v>41223</v>
+        <v>41383</v>
       </c>
       <c r="H11" s="67" t="str">
-        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G11,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 10-Nov-2012</v>
+        <f>"Renewal of Domain and Hosting until "&amp;TEXT(E11,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain and Hosting until 19-Apr-2013</v>
       </c>
       <c r="I11" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B11&amp;" until "&amp;TEXT(G11,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain westcoastexpress.net until 10-Nov-2012</v>
-      </c>
-      <c r="J11" s="68" t="s">
-        <v>40</v>
-      </c>
-      <c r="K11" s="59"/>
-      <c r="L11" s="63" t="s">
-        <v>61</v>
-      </c>
-      <c r="M11" s="63" t="s">
-        <v>86</v>
+        <f>"Renewal of Domain "&amp;B11&amp;" until "&amp;TEXT(E11,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain loviesyarn.com until 19-Apr-2013</v>
       </c>
       <c r="N11" s="63" t="s">
-        <v>102</v>
-      </c>
-      <c r="O11" s="63" t="s">
-        <v>95</v>
-      </c>
-      <c r="P11" s="77"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A12" s="64">
-        <v>1010</v>
+        <v>1002</v>
       </c>
       <c r="B12" s="63" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="C12" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="63" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="78">
-        <v>41283</v>
-      </c>
-      <c r="F12" s="69">
-        <v>131</v>
-      </c>
-      <c r="G12" s="78">
-        <v>41283</v>
+      <c r="D12" s="64" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="66">
+        <v>41399</v>
+      </c>
+      <c r="F12" s="82">
+        <v>198</v>
+      </c>
+      <c r="G12" s="66">
+        <v>41399</v>
       </c>
       <c r="H12" s="67" t="str">
-        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G12,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 09-Jan-2013</v>
+        <f>"Renewal of Domain and Hosting until "&amp;TEXT(E12,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain and Hosting until 05-May-2013</v>
       </c>
       <c r="I12" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B12&amp;" until "&amp;TEXT(G12,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain onestopaberdeen.com until 09-Jan-2013</v>
+        <f>"Renewal of Domain "&amp;B12&amp;" until "&amp;TEXT(E12,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain asrc.biz until 05-May-2013</v>
       </c>
       <c r="J12" s="68" t="s">
         <v>40</v>
       </c>
       <c r="K12" s="59"/>
       <c r="L12" s="63" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="M12" s="63" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="N12" s="63" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="O12" s="63" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A13" s="64">
-        <v>1001</v>
-      </c>
-      <c r="B13" s="63" t="s">
-        <v>17</v>
+        <v>1031</v>
+      </c>
+      <c r="B13" s="83" t="s">
+        <v>143</v>
       </c>
       <c r="C13" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="76">
-        <v>40965</v>
-      </c>
-      <c r="F13" s="74">
-        <v>188</v>
-      </c>
-      <c r="G13" s="76">
-        <v>41331</v>
+      <c r="D13" s="83" t="s">
+        <v>143</v>
+      </c>
+      <c r="E13" s="66">
+        <v>41806</v>
+      </c>
+      <c r="F13" s="82">
+        <v>195</v>
+      </c>
+      <c r="G13" s="66">
+        <v>41441</v>
       </c>
       <c r="H13" s="67" t="str">
-        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G13,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 26-Feb-2013</v>
+        <f>"Renewal of Domain and Hosting until "&amp;TEXT(E13,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain and Hosting until 16-Jun-2014</v>
       </c>
       <c r="I13" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B13&amp;" until "&amp;TEXT(G13,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain relaxatub.com until 26-Feb-2013</v>
-      </c>
-      <c r="J13" s="68" t="s">
-        <v>40</v>
-      </c>
-      <c r="K13" s="59"/>
-      <c r="L13" s="63" t="s">
-        <v>58</v>
-      </c>
-      <c r="M13" s="63" t="s">
-        <v>70</v>
-      </c>
-      <c r="N13" s="63" t="s">
+        <f>"Renewal of Domain "&amp;B13&amp;" until "&amp;TEXT(E13,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain loviesdrapery.co.uk  until 16-Jun-2014</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A14" s="64">
+        <v>1021</v>
+      </c>
+      <c r="B14" s="63" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="65" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="63" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="67">
+        <v>41481</v>
+      </c>
+      <c r="F14" s="82">
+        <v>20114</v>
+      </c>
+      <c r="G14" s="67">
+        <v>41481</v>
+      </c>
+      <c r="H14" s="67" t="str">
+        <f>"Renewal of Domain and Hosting until "&amp;TEXT(E14,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain and Hosting until 26-Jul-2013</v>
+      </c>
+      <c r="I14" s="67" t="str">
+        <f>"Renewal of Domain "&amp;B14&amp;" until "&amp;TEXT(E14,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain keptiebakery.com until 26-Jul-2013</v>
+      </c>
+      <c r="J14" s="68" t="s">
+        <v>40</v>
+      </c>
+      <c r="K14" s="59"/>
+      <c r="L14" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="N14" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="O13" s="63" t="s">
+      <c r="O14" s="63" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="64">
-        <v>1001</v>
-      </c>
-      <c r="B14" s="63" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="65" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="76">
-        <v>41331</v>
-      </c>
-      <c r="F14" s="74">
-        <v>138</v>
-      </c>
-      <c r="G14" s="76">
-        <v>41331</v>
-      </c>
-      <c r="H14" s="67" t="str">
-        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G14,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 26-Feb-2013</v>
-      </c>
-      <c r="I14" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B14&amp;" until "&amp;TEXT(G14,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain relaxatub.co.uk until 26-Feb-2013</v>
-      </c>
-      <c r="J14" s="68" t="s">
-        <v>40</v>
-      </c>
-      <c r="K14" s="63" t="s">
-        <v>107</v>
-      </c>
-      <c r="L14" s="63" t="s">
-        <v>58</v>
-      </c>
-      <c r="M14" s="63" t="s">
-        <v>70</v>
-      </c>
-      <c r="N14" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="O14" s="63" t="s">
-        <v>93</v>
-      </c>
-      <c r="P14" s="63" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q14" s="63" t="s">
-        <v>97</v>
-      </c>
-      <c r="U14" s="72">
-        <v>38982</v>
-      </c>
-      <c r="V14" s="72">
-        <v>38989</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A15" s="64">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="B15" s="63" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C15" s="65" t="s">
         <v>65</v>
       </c>
       <c r="D15" s="63" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="E15" s="66">
-        <v>41348</v>
-      </c>
-      <c r="F15" s="74">
-        <v>189</v>
+        <v>41588</v>
+      </c>
+      <c r="F15" s="82">
+        <v>204</v>
       </c>
       <c r="G15" s="66">
-        <v>41348</v>
+        <v>41588</v>
       </c>
       <c r="H15" s="67" t="str">
-        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G15,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 15-Mar-2013</v>
+        <f>"Renewal of Domain and Hosting until "&amp;TEXT(E15,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain and Hosting until 10-Nov-2013</v>
       </c>
       <c r="I15" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B15&amp;" until "&amp;TEXT(G15,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain airylea.com until 15-Mar-2013</v>
+        <f>"Renewal of Domain "&amp;B15&amp;" until "&amp;TEXT(E15,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain westcoastexpress.net until 10-Nov-2013</v>
       </c>
       <c r="J15" s="68" t="s">
         <v>40</v>
       </c>
       <c r="K15" s="59"/>
       <c r="L15" s="63" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="M15" s="63" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="N15" s="63" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="O15" s="63" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="P15" s="77"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A16" s="64">
-        <v>1020</v>
+        <v>1001</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C16" s="65" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D16" s="63" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="66">
-        <v>41351</v>
-      </c>
-      <c r="F16" s="74">
-        <v>189</v>
-      </c>
-      <c r="G16" s="66">
-        <v>41348</v>
+        <v>17</v>
+      </c>
+      <c r="E16" s="76">
+        <v>41696</v>
+      </c>
+      <c r="F16" s="82">
+        <v>203</v>
+      </c>
+      <c r="G16" s="76">
+        <v>41696</v>
       </c>
       <c r="H16" s="67" t="str">
-        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G16,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 15-Mar-2013</v>
+        <f>"Renewal of Domain and Hosting until "&amp;TEXT(E16,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain and Hosting until 26-Feb-2014</v>
       </c>
       <c r="I16" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B16&amp;" until "&amp;TEXT(G16,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain airyleamotors.com until 15-Mar-2013</v>
+        <f>"Renewal of Domain "&amp;B16&amp;" until "&amp;TEXT(E16,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain relaxatub.com until 26-Feb-2014</v>
       </c>
       <c r="J16" s="68" t="s">
         <v>40</v>
       </c>
       <c r="K16" s="59"/>
       <c r="L16" s="63" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="M16" s="63" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="N16" s="63" t="s">
         <v>94</v>
@@ -1939,45 +1885,45 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A17" s="64">
-        <v>1007</v>
+        <v>1020</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C17" s="65" t="s">
         <v>65</v>
       </c>
       <c r="D17" s="63" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="76">
-        <v>41357</v>
-      </c>
-      <c r="F17" s="83">
-        <v>194</v>
-      </c>
-      <c r="G17" s="76">
-        <v>41357</v>
+        <v>3</v>
+      </c>
+      <c r="E17" s="66">
+        <v>41713</v>
+      </c>
+      <c r="F17" s="82">
+        <v>202</v>
+      </c>
+      <c r="G17" s="66">
+        <v>41713</v>
       </c>
       <c r="H17" s="67" t="str">
-        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G17,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 24-Mar-2013</v>
+        <f>"Renewal of Domain and Hosting until "&amp;TEXT(E17,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain and Hosting until 15-Mar-2014</v>
       </c>
       <c r="I17" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B17&amp;" until "&amp;TEXT(G17,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain dsglasscraft.com until 24-Mar-2013</v>
+        <f>"Renewal of Domain "&amp;B17&amp;" until "&amp;TEXT(E17,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain airylea.com until 15-Mar-2014</v>
       </c>
       <c r="J17" s="68" t="s">
         <v>40</v>
       </c>
       <c r="K17" s="59"/>
       <c r="L17" s="63" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M17" s="63" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N17" s="63" t="s">
         <v>94</v>
@@ -1986,45 +1932,45 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A18" s="64">
-        <v>1004</v>
+        <v>1020</v>
       </c>
       <c r="B18" s="63" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C18" s="65" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D18" s="63" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="67">
-        <v>41096</v>
-      </c>
-      <c r="F18" s="74">
-        <v>191</v>
+        <v>3</v>
+      </c>
+      <c r="E18" s="66">
+        <v>41716</v>
+      </c>
+      <c r="F18" s="82">
+        <v>202</v>
       </c>
       <c r="G18" s="66">
-        <v>41364</v>
+        <v>41713</v>
       </c>
       <c r="H18" s="67" t="str">
-        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G18,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 31-Mar-2013</v>
+        <f>"Renewal of Domain and Hosting until "&amp;TEXT(E18,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain and Hosting until 18-Mar-2014</v>
       </c>
       <c r="I18" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B18&amp;" until "&amp;TEXT(G18,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain midwestmarketforce.com until 31-Mar-2013</v>
+        <f>"Renewal of Domain "&amp;B18&amp;" until "&amp;TEXT(E18,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain airyleamotors.com until 18-Mar-2014</v>
       </c>
       <c r="J18" s="68" t="s">
         <v>40</v>
       </c>
       <c r="K18" s="59"/>
       <c r="L18" s="63" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="M18" s="63" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="N18" s="63" t="s">
         <v>94</v>
@@ -2033,437 +1979,449 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A19" s="64">
-        <v>1004</v>
+        <v>1020</v>
       </c>
       <c r="B19" s="63" t="s">
-        <v>33</v>
+        <v>122</v>
       </c>
       <c r="C19" s="65" t="s">
         <v>66</v>
       </c>
       <c r="D19" s="63" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="66">
-        <v>41116</v>
+        <v>3</v>
+      </c>
+      <c r="E19" s="67">
+        <v>41990</v>
       </c>
       <c r="F19" s="74">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G19" s="66">
-        <v>41364</v>
+        <v>41713</v>
       </c>
       <c r="H19" s="67" t="str">
-        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G19,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 31-Mar-2013</v>
+        <f>"Renewal of Domain and Hosting until "&amp;TEXT(E19,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain and Hosting until 17-Dec-2014</v>
       </c>
       <c r="I19" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B19&amp;" until "&amp;TEXT(G19,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain midwestmarketforce.info until 31-Mar-2013</v>
+        <f>"Renewal of Domain "&amp;B19&amp;" until "&amp;TEXT(E19,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain airylea.co.uk until 17-Dec-2014</v>
       </c>
       <c r="J19" s="68" t="s">
         <v>40</v>
       </c>
       <c r="K19" s="59"/>
       <c r="L19" s="63" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="M19" s="63" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="N19" s="63" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="O19" s="63" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A20" s="64">
+        <v>1004</v>
+      </c>
+      <c r="B20" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="65" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="75">
+        <v>41165</v>
+      </c>
+      <c r="F20" s="74">
+        <v>191</v>
+      </c>
+      <c r="G20" s="66">
+        <v>41729</v>
+      </c>
+      <c r="H20" s="67" t="str">
+        <f>"Renewal of Domain and Hosting until "&amp;TEXT(E20,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain and Hosting until 13-Sep-2012</v>
+      </c>
+      <c r="I20" s="67" t="str">
+        <f>"Renewal of Domain "&amp;B20&amp;" until "&amp;TEXT(E20,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain mwmf.co.uk until 13-Sep-2012</v>
+      </c>
+      <c r="J20" s="68" t="s">
+        <v>40</v>
+      </c>
+      <c r="K20" s="63" t="s">
+        <v>116</v>
+      </c>
+      <c r="L20" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="M20" s="63" t="s">
+        <v>73</v>
+      </c>
+      <c r="N20" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="O20" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="P20" s="63" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q20" s="63" t="s">
+        <v>99</v>
+      </c>
+      <c r="R20" s="63">
+        <v>3528228</v>
+      </c>
+      <c r="S20" s="79" t="s">
+        <v>113</v>
+      </c>
+      <c r="T20" s="79" t="s">
+        <v>115</v>
+      </c>
+      <c r="U20" s="72">
+        <v>38982</v>
+      </c>
+      <c r="V20" s="72">
+        <v>38989</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A21" s="64">
+        <v>1004</v>
+      </c>
+      <c r="B21" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="65" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="66">
+        <v>40999</v>
+      </c>
+      <c r="F21" s="74">
+        <v>191</v>
+      </c>
+      <c r="G21" s="66">
+        <v>41729</v>
+      </c>
+      <c r="H21" s="67" t="str">
+        <f>"Renewal of Domain and Hosting until "&amp;TEXT(E21,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain and Hosting until 31-Mar-2012</v>
+      </c>
+      <c r="I21" s="67" t="str">
+        <f>"Renewal of Domain "&amp;B21&amp;" until "&amp;TEXT(E21,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain filtra.co.uk until 31-Mar-2012</v>
+      </c>
+      <c r="J21" s="68" t="s">
+        <v>40</v>
+      </c>
+      <c r="K21" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="L21" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="M21" s="63" t="s">
+        <v>73</v>
+      </c>
+      <c r="N21" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="O21" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="P21" s="63" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q21" s="63" t="s">
+        <v>99</v>
+      </c>
+      <c r="R21" s="63">
+        <v>3528228</v>
+      </c>
+      <c r="S21" s="79" t="s">
+        <v>113</v>
+      </c>
+      <c r="T21" s="79" t="s">
+        <v>115</v>
+      </c>
+      <c r="U21" s="72">
+        <v>38982</v>
+      </c>
+      <c r="V21" s="72">
+        <v>38989</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A22" s="64">
+        <v>1004</v>
+      </c>
+      <c r="B22" s="63" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="65" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="66">
+        <v>41018</v>
+      </c>
+      <c r="F22" s="74">
+        <v>191</v>
+      </c>
+      <c r="G22" s="66">
+        <v>41729</v>
+      </c>
+      <c r="H22" s="67" t="str">
+        <f>"Renewal of Domain and Hosting until "&amp;TEXT(E22,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain and Hosting until 19-Apr-2012</v>
+      </c>
+      <c r="I22" s="67" t="str">
+        <f>"Renewal of Domain "&amp;B22&amp;" until "&amp;TEXT(E22,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain midwestmarketforce.co.uk until 19-Apr-2012</v>
+      </c>
+      <c r="J22" s="68" t="s">
+        <v>40</v>
+      </c>
+      <c r="K22" s="80" t="s">
+        <v>106</v>
+      </c>
+      <c r="L22" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="M22" s="63" t="s">
+        <v>73</v>
+      </c>
+      <c r="N22" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="O22" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="P22" s="63" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q22" s="63" t="s">
+        <v>99</v>
+      </c>
+      <c r="R22" s="63">
+        <v>3528228</v>
+      </c>
+      <c r="S22" s="79" t="s">
+        <v>113</v>
+      </c>
+      <c r="T22" s="79" t="s">
+        <v>115</v>
+      </c>
+      <c r="U22" s="72">
+        <v>38982</v>
+      </c>
+      <c r="V22" s="72">
+        <v>38989</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="A23" s="64">
         <v>1032</v>
       </c>
-      <c r="B20" s="63" t="s">
+      <c r="B23" s="63" t="s">
+        <v>145</v>
+      </c>
+      <c r="C23" s="65" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="63" t="s">
         <v>144</v>
       </c>
-      <c r="C20" s="65" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="63" t="s">
-        <v>144</v>
-      </c>
-      <c r="E20" s="66">
-        <v>41383</v>
-      </c>
-      <c r="F20" s="83">
+      <c r="E23" s="66">
+        <v>41748</v>
+      </c>
+      <c r="F23" s="82">
         <v>193</v>
       </c>
-      <c r="G20" s="66">
-        <v>41383</v>
-      </c>
-      <c r="H20" s="67" t="str">
-        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G20,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 19-Apr-2013</v>
-      </c>
-      <c r="I20" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B20&amp;" until "&amp;TEXT(G20,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain loviesyarn.com until 19-Apr-2013</v>
-      </c>
-      <c r="N20" s="63" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="64">
-        <v>1002</v>
-      </c>
-      <c r="B21" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="65" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" s="64" t="s">
-        <v>67</v>
-      </c>
-      <c r="E21" s="66">
-        <v>41399</v>
-      </c>
-      <c r="F21" s="83">
-        <v>198</v>
-      </c>
-      <c r="G21" s="66">
-        <v>41399</v>
-      </c>
-      <c r="H21" s="67" t="str">
-        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G21,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 05-May-2013</v>
-      </c>
-      <c r="I21" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B21&amp;" until "&amp;TEXT(G21,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain asrc.biz until 05-May-2013</v>
-      </c>
-      <c r="J21" s="68" t="s">
-        <v>40</v>
-      </c>
-      <c r="K21" s="59"/>
-      <c r="L21" s="63" t="s">
-        <v>68</v>
-      </c>
-      <c r="M21" s="63" t="s">
-        <v>71</v>
-      </c>
-      <c r="N21" s="63" t="s">
-        <v>100</v>
-      </c>
-      <c r="O21" s="63" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" s="64">
-        <v>1031</v>
-      </c>
-      <c r="B22" s="84" t="s">
-        <v>143</v>
-      </c>
-      <c r="C22" s="65" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" s="84" t="s">
-        <v>143</v>
-      </c>
-      <c r="E22" s="66">
-        <v>41806</v>
-      </c>
-      <c r="F22" s="83">
-        <v>195</v>
-      </c>
-      <c r="G22" s="66">
-        <v>41441</v>
-      </c>
-      <c r="H22" s="67" t="str">
-        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G22,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 16-Jun-2013</v>
-      </c>
-      <c r="I22" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B22&amp;" until "&amp;TEXT(G22,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain loviesdrapery.co.uk  until 16-Jun-2013</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="64">
-        <v>1021</v>
-      </c>
-      <c r="B23" s="63" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="65" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" s="63" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="67">
-        <v>41481</v>
-      </c>
-      <c r="F23" s="83">
-        <v>20114</v>
-      </c>
-      <c r="G23" s="67">
-        <v>41481</v>
+      <c r="G23" s="66">
+        <v>41748</v>
       </c>
       <c r="H23" s="67" t="str">
-        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G23,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 26-Jul-2013</v>
+        <f>"Renewal of Domain and Hosting until "&amp;TEXT(E23,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain and Hosting until 19-Apr-2014</v>
       </c>
       <c r="I23" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B23&amp;" until "&amp;TEXT(G23,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain keptiebakery.com until 26-Jul-2013</v>
-      </c>
-      <c r="J23" s="68" t="s">
-        <v>40</v>
-      </c>
-      <c r="K23" s="59"/>
-      <c r="L23" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="N23" s="63" t="s">
-        <v>94</v>
-      </c>
-      <c r="O23" s="63" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+        <f>"Renewal of Domain "&amp;B23&amp;" until "&amp;TEXT(E23,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain loviesyarn.co.uk until 19-Apr-2014</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A24" s="64">
-        <v>1020</v>
+        <v>1001</v>
       </c>
       <c r="B24" s="63" t="s">
-        <v>122</v>
+        <v>37</v>
       </c>
       <c r="C24" s="65" t="s">
         <v>66</v>
       </c>
       <c r="D24" s="63" t="s">
-        <v>3</v>
-      </c>
-      <c r="E24" s="67">
-        <v>41625</v>
-      </c>
-      <c r="F24" s="74">
-        <v>189</v>
-      </c>
-      <c r="G24" s="66">
-        <v>41713</v>
+        <v>17</v>
+      </c>
+      <c r="E24" s="76">
+        <v>42061</v>
+      </c>
+      <c r="F24" s="82">
+        <v>203</v>
+      </c>
+      <c r="G24" s="76">
+        <v>42061</v>
       </c>
       <c r="H24" s="67" t="str">
-        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G24,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 15-Mar-2014</v>
+        <f>"Renewal of Domain and Hosting until "&amp;TEXT(E24,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain and Hosting until 26-Feb-2015</v>
       </c>
       <c r="I24" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B24&amp;" until "&amp;TEXT(G24,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain airylea.co.uk until 15-Mar-2014</v>
+        <f>"Renewal of Domain "&amp;B24&amp;" until "&amp;TEXT(E24,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain relaxatub.co.uk until 26-Feb-2015</v>
       </c>
       <c r="J24" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="K24" s="59"/>
+      <c r="K24" s="63" t="s">
+        <v>107</v>
+      </c>
       <c r="L24" s="63" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="M24" s="63" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="N24" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="O24" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="P24" s="63" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q24" s="63" t="s">
+        <v>97</v>
+      </c>
+      <c r="U24" s="72">
+        <v>38982</v>
+      </c>
+      <c r="V24" s="72">
+        <v>38989</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="B25" s="63" t="s">
+        <v>135</v>
+      </c>
+      <c r="C25" s="65" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="64" t="s">
+        <v>135</v>
+      </c>
+      <c r="E25" s="75">
+        <v>40869</v>
+      </c>
+      <c r="G25" s="75"/>
+      <c r="H25" s="67" t="str">
+        <f>"Renewal of Domain and Hosting until "&amp;TEXT(E25,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain and Hosting until 22-Nov-2011</v>
+      </c>
+      <c r="I25" s="67" t="str">
+        <f>"Renewal of Domain "&amp;B25&amp;" until "&amp;TEXT(E25,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain andoverprimary.org until 22-Nov-2011</v>
+      </c>
+      <c r="J25" s="68" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.45">
+      <c r="B26" s="63" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="65" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="63" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="78">
+        <v>39407</v>
+      </c>
+      <c r="F26" s="69"/>
+      <c r="G26" s="69"/>
+      <c r="H26" s="67" t="str">
+        <f>"Renewal of Domain and Hosting until "&amp;TEXT(E26,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain and Hosting until 21-Nov-2007</v>
+      </c>
+      <c r="I26" s="67" t="str">
+        <f>"Renewal of Domain "&amp;B26&amp;" until "&amp;TEXT(E26,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain southesk.com until 21-Nov-2007</v>
+      </c>
+      <c r="J26" s="68" t="s">
+        <v>40</v>
+      </c>
+      <c r="K26" s="59"/>
+      <c r="L26" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="N26" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="O24" s="63" t="s">
+      <c r="O26" s="63" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="64">
-        <v>1004</v>
-      </c>
-      <c r="B25" s="63" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="65" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" s="63" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="75">
-        <v>41165</v>
-      </c>
-      <c r="F25" s="74">
-        <v>191</v>
-      </c>
-      <c r="G25" s="66">
-        <v>41729</v>
-      </c>
-      <c r="H25" s="67" t="str">
-        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G25,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 31-Mar-2014</v>
-      </c>
-      <c r="I25" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B25&amp;" until "&amp;TEXT(G25,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain mwmf.co.uk until 31-Mar-2014</v>
-      </c>
-      <c r="J25" s="68" t="s">
-        <v>40</v>
-      </c>
-      <c r="K25" s="63" t="s">
-        <v>116</v>
-      </c>
-      <c r="L25" s="63" t="s">
-        <v>54</v>
-      </c>
-      <c r="M25" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="N25" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="O25" s="63" t="s">
-        <v>93</v>
-      </c>
-      <c r="P25" s="63" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q25" s="63" t="s">
-        <v>99</v>
-      </c>
-      <c r="R25" s="63">
-        <v>3528228</v>
-      </c>
-      <c r="S25" s="79" t="s">
-        <v>113</v>
-      </c>
-      <c r="T25" s="79" t="s">
-        <v>115</v>
-      </c>
-      <c r="U25" s="72">
-        <v>38982</v>
-      </c>
-      <c r="V25" s="72">
-        <v>38989</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A26" s="64">
-        <v>1004</v>
-      </c>
-      <c r="B26" s="63" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="65" t="s">
-        <v>66</v>
-      </c>
-      <c r="D26" s="63" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="66">
-        <v>40999</v>
-      </c>
-      <c r="F26" s="74">
-        <v>191</v>
-      </c>
-      <c r="G26" s="66">
-        <v>41729</v>
-      </c>
-      <c r="H26" s="67" t="str">
-        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G26,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 31-Mar-2014</v>
-      </c>
-      <c r="I26" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B26&amp;" until "&amp;TEXT(G26,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain filtra.co.uk until 31-Mar-2014</v>
-      </c>
-      <c r="J26" s="68" t="s">
-        <v>40</v>
-      </c>
-      <c r="K26" s="63" t="s">
-        <v>110</v>
-      </c>
-      <c r="L26" s="63" t="s">
-        <v>54</v>
-      </c>
-      <c r="M26" s="63" t="s">
-        <v>73</v>
-      </c>
-      <c r="N26" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="O26" s="63" t="s">
-        <v>93</v>
-      </c>
-      <c r="P26" s="63" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q26" s="63" t="s">
-        <v>99</v>
-      </c>
-      <c r="R26" s="63">
-        <v>3528228</v>
-      </c>
-      <c r="S26" s="79" t="s">
-        <v>113</v>
-      </c>
-      <c r="T26" s="79" t="s">
-        <v>115</v>
-      </c>
-      <c r="U26" s="72">
-        <v>38982</v>
-      </c>
-      <c r="V26" s="72">
-        <v>38989</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" s="64">
-        <v>1004</v>
-      </c>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.45">
       <c r="B27" s="63" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="C27" s="65" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D27" s="63" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" s="66">
-        <v>41018</v>
-      </c>
-      <c r="F27" s="74">
-        <v>191</v>
-      </c>
-      <c r="G27" s="66">
-        <v>41729</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="E27" s="78">
+        <v>39452</v>
+      </c>
+      <c r="F27" s="69"/>
+      <c r="G27" s="69"/>
       <c r="H27" s="67" t="str">
-        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G27,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 31-Mar-2014</v>
+        <f>"Renewal of Domain and Hosting until "&amp;TEXT(E27,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain and Hosting until 05-Jan-2008</v>
       </c>
       <c r="I27" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B27&amp;" until "&amp;TEXT(G27,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain midwestmarketforce.co.uk until 31-Mar-2014</v>
+        <f>"Renewal of Domain "&amp;B27&amp;" until "&amp;TEXT(E27,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain frontburner.co.uk until 05-Jan-2008</v>
       </c>
       <c r="J27" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="K27" s="80" t="s">
-        <v>106</v>
+      <c r="K27" s="63" t="s">
+        <v>119</v>
       </c>
       <c r="L27" s="63" t="s">
-        <v>54</v>
-      </c>
-      <c r="M27" s="63" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="N27" s="63" t="s">
         <v>92</v>
@@ -2472,176 +2430,22 @@
         <v>93</v>
       </c>
       <c r="P27" s="63" t="s">
-        <v>98</v>
+        <v>49</v>
       </c>
       <c r="Q27" s="63" t="s">
-        <v>99</v>
-      </c>
-      <c r="R27" s="63">
-        <v>3528228</v>
-      </c>
-      <c r="S27" s="79" t="s">
-        <v>113</v>
-      </c>
-      <c r="T27" s="79" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="U27" s="72">
-        <v>38982</v>
+        <v>38985</v>
       </c>
       <c r="V27" s="72">
         <v>38989</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A28" s="64">
-        <v>1032</v>
-      </c>
-      <c r="B28" s="63" t="s">
-        <v>145</v>
-      </c>
-      <c r="C28" s="65" t="s">
-        <v>66</v>
-      </c>
-      <c r="D28" s="63" t="s">
-        <v>144</v>
-      </c>
-      <c r="E28" s="66">
-        <v>41748</v>
-      </c>
-      <c r="F28" s="83">
-        <v>193</v>
-      </c>
-      <c r="G28" s="66">
-        <v>41748</v>
-      </c>
-      <c r="H28" s="67" t="str">
-        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G28,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 19-Apr-2014</v>
-      </c>
-      <c r="I28" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B28&amp;" until "&amp;TEXT(G28,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain loviesyarn.co.uk until 19-Apr-2014</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B29" s="63" t="s">
-        <v>135</v>
-      </c>
-      <c r="C29" s="65" t="s">
-        <v>65</v>
-      </c>
-      <c r="D29" s="64" t="s">
-        <v>135</v>
-      </c>
-      <c r="E29" s="75">
-        <v>40869</v>
-      </c>
-      <c r="G29" s="75"/>
-      <c r="H29" s="67" t="str">
-        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G29,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 00-Jan-1900</v>
-      </c>
-      <c r="I29" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B29&amp;" until "&amp;TEXT(G29,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain andoverprimary.org until 00-Jan-1900</v>
-      </c>
-      <c r="J29" s="68" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B30" s="63" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30" s="65" t="s">
-        <v>65</v>
-      </c>
-      <c r="D30" s="63" t="s">
-        <v>18</v>
-      </c>
-      <c r="E30" s="78">
-        <v>39407</v>
-      </c>
-      <c r="F30" s="69"/>
-      <c r="G30" s="69"/>
-      <c r="H30" s="67" t="str">
-        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G30,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 00-Jan-1900</v>
-      </c>
-      <c r="I30" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B30&amp;" until "&amp;TEXT(G30,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain southesk.com until 00-Jan-1900</v>
-      </c>
-      <c r="J30" s="68" t="s">
-        <v>40</v>
-      </c>
-      <c r="K30" s="59"/>
-      <c r="L30" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="N30" s="63" t="s">
-        <v>94</v>
-      </c>
-      <c r="O30" s="63" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B31" s="63" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" s="65" t="s">
-        <v>65</v>
-      </c>
-      <c r="D31" s="63" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="78">
-        <v>39452</v>
-      </c>
-      <c r="F31" s="69"/>
-      <c r="G31" s="69"/>
-      <c r="H31" s="67" t="str">
-        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G31,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain and Hosting until 00-Jan-1900</v>
-      </c>
-      <c r="I31" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B31&amp;" until "&amp;TEXT(G31,"dd-MMM-yyyy")</f>
-        <v>Renewal of Domain frontburner.co.uk until 00-Jan-1900</v>
-      </c>
-      <c r="J31" s="68" t="s">
-        <v>40</v>
-      </c>
-      <c r="K31" s="63" t="s">
-        <v>119</v>
-      </c>
-      <c r="L31" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="N31" s="63" t="s">
-        <v>92</v>
-      </c>
-      <c r="O31" s="63" t="s">
-        <v>93</v>
-      </c>
-      <c r="P31" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q31" s="63" t="s">
-        <v>97</v>
-      </c>
-      <c r="U31" s="72">
-        <v>38985</v>
-      </c>
-      <c r="V31" s="72">
-        <v>38989</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:L27"/>
-  <sortState ref="A2:V31">
-    <sortCondition ref="G2:G31"/>
+  <autoFilter ref="A1:L23"/>
+  <sortState ref="A2:V27">
+    <sortCondition ref="G2:G27"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2658,30 +2462,30 @@
       <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.85" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.3984375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.1328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.86328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -2740,7 +2544,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.4">
       <c r="A2" s="4">
         <v>1011</v>
       </c>
@@ -2779,7 +2583,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.4">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
         <v>129</v>
@@ -2802,7 +2606,7 @@
       </c>
       <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.4">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
         <v>130</v>
@@ -2825,7 +2629,7 @@
       </c>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.4">
       <c r="A5" s="4">
         <v>1011</v>
       </c>
@@ -2873,37 +2677,37 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V23"/>
+  <dimension ref="A1:V27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+      <selection activeCell="A24" sqref="A24:XFD27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.85" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.1328125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="26" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="57.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="57.1328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.86328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.3984375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.86328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -2962,7 +2766,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" s="35" customFormat="1" ht="13.2" x14ac:dyDescent="0.4">
       <c r="A2" s="34">
         <v>1014</v>
       </c>
@@ -2997,7 +2801,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" s="14" customFormat="1" ht="13.2" x14ac:dyDescent="0.4">
       <c r="A3" s="34"/>
       <c r="B3" s="35" t="s">
         <v>4</v>
@@ -3045,7 +2849,7 @@
         <v>38989</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.4">
       <c r="A4" s="34">
         <v>1005</v>
       </c>
@@ -3087,7 +2891,7 @@
       <c r="S4" s="35"/>
       <c r="T4" s="35"/>
     </row>
-    <row r="5" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.4">
       <c r="A5" s="7">
         <v>1004</v>
       </c>
@@ -3120,7 +2924,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.4">
       <c r="A6" s="15">
         <v>1008</v>
       </c>
@@ -3162,7 +2966,7 @@
       <c r="S6" s="16"/>
       <c r="T6" s="16"/>
     </row>
-    <row r="7" spans="1:20" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" s="46" customFormat="1" ht="13.2" x14ac:dyDescent="0.4">
       <c r="A7" s="45"/>
       <c r="B7" s="46" t="s">
         <v>29</v>
@@ -3194,7 +2998,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:20" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" s="44" customFormat="1" ht="13.2" x14ac:dyDescent="0.4">
       <c r="A8" s="51">
         <v>1004</v>
       </c>
@@ -3233,7 +3037,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.4">
       <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
         <v>7</v>
@@ -3279,7 +3083,7 @@
         <v>38989</v>
       </c>
     </row>
-    <row r="10" spans="1:20" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.4">
       <c r="A10" s="4">
         <v>1003</v>
       </c>
@@ -3325,7 +3129,7 @@
       <c r="S10" s="5"/>
       <c r="T10" s="5"/>
     </row>
-    <row r="11" spans="1:20" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" s="33" customFormat="1" ht="13.2" x14ac:dyDescent="0.4">
       <c r="A11" s="4">
         <v>1009</v>
       </c>
@@ -3371,7 +3175,7 @@
       <c r="S11" s="5"/>
       <c r="T11" s="5"/>
     </row>
-    <row r="12" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.4">
       <c r="A12" s="4">
         <v>1009</v>
       </c>
@@ -3420,7 +3224,7 @@
         <v>38989</v>
       </c>
     </row>
-    <row r="13" spans="1:20" s="43" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" s="43" customFormat="1" ht="13.2" x14ac:dyDescent="0.4">
       <c r="A13" s="4">
         <v>1000</v>
       </c>
@@ -3466,7 +3270,7 @@
       <c r="S13" s="5"/>
       <c r="T13" s="5"/>
     </row>
-    <row r="14" spans="1:20" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" s="44" customFormat="1" ht="13.2" x14ac:dyDescent="0.4">
       <c r="A14" s="4">
         <v>1000</v>
       </c>
@@ -3512,7 +3316,7 @@
       <c r="S14" s="5"/>
       <c r="T14" s="5"/>
     </row>
-    <row r="15" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.4">
       <c r="A15" s="4">
         <v>1000</v>
       </c>
@@ -3559,7 +3363,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.4">
       <c r="A16" s="4">
         <v>1000</v>
       </c>
@@ -3606,7 +3410,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.4">
       <c r="A17" s="4">
         <v>1025</v>
       </c>
@@ -3633,7 +3437,7 @@
       </c>
       <c r="I17" s="13"/>
     </row>
-    <row r="18" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.4">
       <c r="A18" s="4">
         <v>1025</v>
       </c>
@@ -3664,7 +3468,7 @@
       </c>
       <c r="J18" s="13"/>
     </row>
-    <row r="19" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.4">
       <c r="A19" s="4">
         <v>1027</v>
       </c>
@@ -3695,7 +3499,7 @@
       </c>
       <c r="J19" s="13"/>
     </row>
-    <row r="20" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.4">
       <c r="A20" s="4">
         <v>1026</v>
       </c>
@@ -3726,7 +3530,7 @@
       </c>
       <c r="J20" s="13"/>
     </row>
-    <row r="21" spans="1:22" s="63" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" s="63" customFormat="1" ht="14.35" x14ac:dyDescent="0.45">
       <c r="A21" s="64">
         <v>1012</v>
       </c>
@@ -3742,7 +3546,7 @@
       <c r="E21" s="73">
         <v>40791</v>
       </c>
-      <c r="F21" s="83">
+      <c r="F21" s="82">
         <v>20116</v>
       </c>
       <c r="G21" s="73">
@@ -3753,7 +3557,7 @@
         <v>Renewal of Domain and Hosting until 05-Sep-2011</v>
       </c>
       <c r="I21" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B21&amp;" until "&amp;TEXT(G21,"dd-MMM-yyyy")</f>
+        <f t="shared" ref="I21:I27" si="1">"Renewal of Domain "&amp;B21&amp;" until "&amp;TEXT(G21,"dd-MMM-yyyy")</f>
         <v>Renewal of Domain partnersinlearning.org.uk until 05-Sep-2011</v>
       </c>
       <c r="J21" s="68" t="s">
@@ -3787,7 +3591,7 @@
         <v>38989</v>
       </c>
     </row>
-    <row r="22" spans="1:22" s="63" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" s="63" customFormat="1" ht="14.35" x14ac:dyDescent="0.45">
       <c r="A22" s="64">
         <v>1018</v>
       </c>
@@ -3803,7 +3607,7 @@
       <c r="E22" s="76">
         <v>40855</v>
       </c>
-      <c r="F22" s="83">
+      <c r="F22" s="82">
         <v>20120</v>
       </c>
       <c r="G22" s="76">
@@ -3814,7 +3618,7 @@
         <v>Renewal of Domain and Hosting until 08-Nov-2011</v>
       </c>
       <c r="I22" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B22&amp;" until "&amp;TEXT(G22,"dd-MMM-yyyy")</f>
+        <f t="shared" si="1"/>
         <v>Renewal of Domain earnnow.info until 08-Nov-2011</v>
       </c>
       <c r="J22" s="68" t="s">
@@ -3833,7 +3637,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:22" s="63" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" s="63" customFormat="1" ht="14.35" x14ac:dyDescent="0.45">
       <c r="A23" s="64">
         <v>1032</v>
       </c>
@@ -3849,7 +3653,7 @@
       <c r="E23" s="66">
         <v>41076</v>
       </c>
-      <c r="F23" s="90">
+      <c r="F23" s="89">
         <v>136</v>
       </c>
       <c r="G23" s="66">
@@ -3860,8 +3664,201 @@
         <v>Renewal of Domain and Hosting until 16-Jun-2012</v>
       </c>
       <c r="I23" s="67" t="str">
-        <f>"Renewal of Domain "&amp;B23&amp;" until "&amp;TEXT(G23,"dd-MMM-yyyy")</f>
+        <f t="shared" si="1"/>
         <v>Renewal of Domain iknit.biz until 16-Jun-2012</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" s="63" customFormat="1" ht="14.35" x14ac:dyDescent="0.45">
+      <c r="A24" s="64">
+        <v>1015</v>
+      </c>
+      <c r="B24" s="63" t="s">
+        <v>137</v>
+      </c>
+      <c r="C24" s="65" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="63" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" s="75">
+        <v>40860</v>
+      </c>
+      <c r="F24" s="82">
+        <v>20113</v>
+      </c>
+      <c r="G24" s="70">
+        <v>41118</v>
+      </c>
+      <c r="H24" s="67" t="str">
+        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G24,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain and Hosting until 28-Jul-2012</v>
+      </c>
+      <c r="I24" s="67" t="str">
+        <f t="shared" si="1"/>
+        <v>Renewal of Domain stourvalleytechnicalservices.co.uk until 28-Jul-2012</v>
+      </c>
+      <c r="J24" s="68" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" s="63" customFormat="1" ht="14.35" x14ac:dyDescent="0.45">
+      <c r="A25" s="64">
+        <v>1015</v>
+      </c>
+      <c r="B25" s="63" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="65" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="63" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="70">
+        <v>41483</v>
+      </c>
+      <c r="F25" s="89">
+        <v>137</v>
+      </c>
+      <c r="G25" s="70">
+        <v>41118</v>
+      </c>
+      <c r="H25" s="67" t="str">
+        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G25,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain and Hosting until 28-Jul-2012</v>
+      </c>
+      <c r="I25" s="67" t="str">
+        <f t="shared" si="1"/>
+        <v>Renewal of Domain stourvalleytimberengineering.co.uk until 28-Jul-2012</v>
+      </c>
+      <c r="J25" s="68" t="s">
+        <v>40</v>
+      </c>
+      <c r="K25" s="63" t="s">
+        <v>118</v>
+      </c>
+      <c r="L25" s="63" t="s">
+        <v>60</v>
+      </c>
+      <c r="M25" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="N25" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="O25" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="P25" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q25" s="63" t="s">
+        <v>97</v>
+      </c>
+      <c r="U25" s="72">
+        <v>38985</v>
+      </c>
+      <c r="V25" s="72">
+        <v>38989</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" s="63" customFormat="1" ht="14.35" x14ac:dyDescent="0.45">
+      <c r="A26" s="64">
+        <v>1015</v>
+      </c>
+      <c r="B26" s="63" t="s">
+        <v>138</v>
+      </c>
+      <c r="C26" s="65" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" s="63" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" s="75">
+        <v>40619</v>
+      </c>
+      <c r="F26" s="89">
+        <v>137</v>
+      </c>
+      <c r="G26" s="70">
+        <v>41118</v>
+      </c>
+      <c r="H26" s="67" t="str">
+        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G26,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain and Hosting until 28-Jul-2012</v>
+      </c>
+      <c r="I26" s="67" t="str">
+        <f t="shared" si="1"/>
+        <v>Renewal of Domain svts.co.uk until 28-Jul-2012</v>
+      </c>
+      <c r="J26" s="68" t="s">
+        <v>40</v>
+      </c>
+      <c r="L26" s="63" t="s">
+        <v>60</v>
+      </c>
+      <c r="M26" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="N26" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="O26" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="P26" s="63" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" s="63" customFormat="1" ht="14.35" x14ac:dyDescent="0.45">
+      <c r="A27" s="64">
+        <v>1015</v>
+      </c>
+      <c r="B27" s="63" t="s">
+        <v>125</v>
+      </c>
+      <c r="C27" s="65" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="63" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="75">
+        <v>40821</v>
+      </c>
+      <c r="F27" s="89">
+        <v>137</v>
+      </c>
+      <c r="G27" s="70">
+        <v>41118</v>
+      </c>
+      <c r="H27" s="67" t="str">
+        <f>"Renewal of Domain and Hosting until "&amp;TEXT(G27,"dd-MMM-yyyy")</f>
+        <v>Renewal of Domain and Hosting until 28-Jul-2012</v>
+      </c>
+      <c r="I27" s="67" t="str">
+        <f t="shared" si="1"/>
+        <v>Renewal of Domain svte.co.uk until 28-Jul-2012</v>
+      </c>
+      <c r="J27" s="68" t="s">
+        <v>40</v>
+      </c>
+      <c r="L27" s="63" t="s">
+        <v>60</v>
+      </c>
+      <c r="M27" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="N27" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="O27" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="P27" s="63" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>